<commit_message>
add raw data from COMPUSTAT and CRSP; merge COMPUSTAT/CRSP/EDGAR
</commit_message>
<xml_diff>
--- a/output/Tables.xlsx
+++ b/output/Tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>count</t>
   </si>
@@ -38,6 +38,75 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>cik</t>
+  </si>
+  <si>
+    <t>gvkey</t>
+  </si>
+  <si>
+    <t>sic</t>
+  </si>
+  <si>
+    <t>fyearq</t>
+  </si>
+  <si>
+    <t>fqtr</t>
+  </si>
+  <si>
+    <t>fyr</t>
+  </si>
+  <si>
+    <t>ipodate</t>
+  </si>
+  <si>
+    <t>exchg</t>
+  </si>
+  <si>
+    <t>actq</t>
+  </si>
+  <si>
+    <t>atq</t>
+  </si>
+  <si>
+    <t>ceqq</t>
+  </si>
+  <si>
+    <t>cheq</t>
+  </si>
+  <si>
+    <t>cshoq</t>
+  </si>
+  <si>
+    <t>dlcq</t>
+  </si>
+  <si>
+    <t>dlttq</t>
+  </si>
+  <si>
+    <t>dpq</t>
+  </si>
+  <si>
+    <t>ibq</t>
+  </si>
+  <si>
+    <t>intanq</t>
+  </si>
+  <si>
+    <t>lctq</t>
+  </si>
+  <si>
+    <t>revtq</t>
+  </si>
+  <si>
+    <t>txditcq</t>
+  </si>
+  <si>
+    <t>prccq</t>
+  </si>
+  <si>
+    <t>RET</t>
   </si>
   <si>
     <t>nw</t>
@@ -431,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,28 +537,28 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>564075</v>
+        <v>300806</v>
       </c>
       <c r="C2">
-        <v>9456.23</v>
+        <v>825241.88</v>
       </c>
       <c r="D2">
-        <v>7330.08</v>
+        <v>431217.67</v>
       </c>
       <c r="E2">
-        <v>890</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>4078</v>
+        <v>722313</v>
       </c>
       <c r="G2">
-        <v>7423</v>
+        <v>897077</v>
       </c>
       <c r="H2">
-        <v>12625</v>
+        <v>1068292</v>
       </c>
       <c r="I2">
-        <v>45537</v>
+        <v>1783400</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -497,28 +566,28 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>564075</v>
+        <v>300806</v>
       </c>
       <c r="C3">
-        <v>1485.95</v>
+        <v>55561.05</v>
       </c>
       <c r="D3">
-        <v>684.9400000000001</v>
+        <v>59534.06</v>
       </c>
       <c r="E3">
-        <v>103</v>
+        <v>1004</v>
       </c>
       <c r="F3">
-        <v>974</v>
+        <v>11506</v>
       </c>
       <c r="G3">
-        <v>1396</v>
+        <v>26071</v>
       </c>
       <c r="H3">
-        <v>1863</v>
+        <v>66288</v>
       </c>
       <c r="I3">
-        <v>12326</v>
+        <v>332115</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -526,28 +595,28 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>564075</v>
+        <v>300806</v>
       </c>
       <c r="C4">
-        <v>148.09</v>
+        <v>4951.72</v>
       </c>
       <c r="D4">
-        <v>170.52</v>
+        <v>1961.91</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F4">
-        <v>42</v>
+        <v>3537</v>
       </c>
       <c r="G4">
-        <v>90</v>
+        <v>4955</v>
       </c>
       <c r="H4">
-        <v>185</v>
+        <v>6351</v>
       </c>
       <c r="I4">
-        <v>2465</v>
+        <v>9997</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -555,28 +624,28 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>564075</v>
+        <v>300806</v>
       </c>
       <c r="C5">
-        <v>55.28</v>
+        <v>2006.47</v>
       </c>
       <c r="D5">
-        <v>56.92</v>
+        <v>7.26</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1993</v>
       </c>
       <c r="F5">
-        <v>18</v>
+        <v>2000</v>
       </c>
       <c r="G5">
-        <v>38</v>
+        <v>2006</v>
       </c>
       <c r="H5">
-        <v>73</v>
+        <v>2013</v>
       </c>
       <c r="I5">
-        <v>722</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -584,28 +653,28 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>564075</v>
+        <v>300775</v>
       </c>
       <c r="C6">
-        <v>126.77</v>
+        <v>2.01</v>
       </c>
       <c r="D6">
-        <v>129.02</v>
+        <v>0.82</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>164</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>1460</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -613,28 +682,28 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>564075</v>
+        <v>300806</v>
       </c>
       <c r="C7">
-        <v>100.04</v>
+        <v>10.39</v>
       </c>
       <c r="D7">
-        <v>152.59</v>
+        <v>3.06</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="H7">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="I7">
-        <v>2851</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -642,28 +711,28 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>564075</v>
+        <v>166792</v>
       </c>
       <c r="C8">
-        <v>63.71</v>
+        <v>19977408.58</v>
       </c>
       <c r="D8">
-        <v>64.95</v>
+        <v>74491.00999999999</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>19680313</v>
       </c>
       <c r="F8">
-        <v>20</v>
+        <v>19930929</v>
       </c>
       <c r="G8">
-        <v>43</v>
+        <v>19961119</v>
       </c>
       <c r="H8">
-        <v>85</v>
+        <v>20000808</v>
       </c>
       <c r="I8">
-        <v>785</v>
+        <v>20191025</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -671,28 +740,28 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>564075</v>
+        <v>300793</v>
       </c>
       <c r="C9">
-        <v>28.15</v>
+        <v>13.5</v>
       </c>
       <c r="D9">
-        <v>28.41</v>
+        <v>2.47</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H9">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="I9">
-        <v>767</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -700,28 +769,28 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>564075</v>
+        <v>228135</v>
       </c>
       <c r="C10">
-        <v>30.22</v>
+        <v>933.17</v>
       </c>
       <c r="D10">
-        <v>28.21</v>
+        <v>4139.53</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>11</v>
+        <v>38.01</v>
       </c>
       <c r="G10">
-        <v>22</v>
+        <v>129.88</v>
       </c>
       <c r="H10">
-        <v>40</v>
+        <v>465.03</v>
       </c>
       <c r="I10">
-        <v>322</v>
+        <v>167633</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -729,28 +798,28 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>564075</v>
+        <v>299687</v>
       </c>
       <c r="C11">
-        <v>49.06</v>
+        <v>6658.01</v>
       </c>
       <c r="D11">
-        <v>74.93000000000001</v>
+        <v>59052.73</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>107.28</v>
       </c>
       <c r="G11">
-        <v>26</v>
+        <v>474.47</v>
       </c>
       <c r="H11">
-        <v>52</v>
+        <v>1961.14</v>
       </c>
       <c r="I11">
-        <v>1038</v>
+        <v>3293755</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -758,28 +827,28 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>564075</v>
+        <v>299140</v>
       </c>
       <c r="C12">
-        <v>3.57</v>
+        <v>1331.75</v>
       </c>
       <c r="D12">
-        <v>7.72</v>
+        <v>7503.48</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>-106362</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>41.65</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>149.62</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>589.89</v>
       </c>
       <c r="I12">
-        <v>203</v>
+        <v>397609</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -787,28 +856,695 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>564075</v>
+        <v>299498</v>
       </c>
       <c r="C13">
+        <v>752.67</v>
+      </c>
+      <c r="D13">
+        <v>10581.1</v>
+      </c>
+      <c r="E13">
+        <v>-26</v>
+      </c>
+      <c r="F13">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="G13">
+        <v>37.27</v>
+      </c>
+      <c r="H13">
+        <v>141.88</v>
+      </c>
+      <c r="I13">
+        <v>748548</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>299502</v>
+      </c>
+      <c r="C14">
+        <v>94.62</v>
+      </c>
+      <c r="D14">
+        <v>386.67</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>10.94</v>
+      </c>
+      <c r="G14">
+        <v>26.42</v>
+      </c>
+      <c r="H14">
+        <v>63.32</v>
+      </c>
+      <c r="I14">
+        <v>29206.44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>274034</v>
+      </c>
+      <c r="C15">
+        <v>643.17</v>
+      </c>
+      <c r="D15">
+        <v>10483.64</v>
+      </c>
+      <c r="E15">
+        <v>-0.09</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>2.81</v>
+      </c>
+      <c r="H15">
+        <v>30.65</v>
+      </c>
+      <c r="I15">
+        <v>519230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>297205</v>
+      </c>
+      <c r="C16">
+        <v>1264.37</v>
+      </c>
+      <c r="D16">
+        <v>13910.54</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>46.25</v>
+      </c>
+      <c r="H16">
+        <v>393.1</v>
+      </c>
+      <c r="I16">
+        <v>3048499</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>267133</v>
+      </c>
+      <c r="C17">
+        <v>30.54</v>
+      </c>
+      <c r="D17">
+        <v>168.87</v>
+      </c>
+      <c r="E17">
+        <v>-33</v>
+      </c>
+      <c r="F17">
+        <v>0.48</v>
+      </c>
+      <c r="G17">
+        <v>2.26</v>
+      </c>
+      <c r="H17">
+        <v>11.77</v>
+      </c>
+      <c r="I17">
+        <v>8166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>299584</v>
+      </c>
+      <c r="C18">
+        <v>40.99</v>
+      </c>
+      <c r="D18">
+        <v>362.35</v>
+      </c>
+      <c r="E18">
+        <v>-41847.9</v>
+      </c>
+      <c r="F18">
+        <v>-0.79</v>
+      </c>
+      <c r="G18">
+        <v>2.1</v>
+      </c>
+      <c r="H18">
+        <v>14.72</v>
+      </c>
+      <c r="I18">
+        <v>22628</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>212759</v>
+      </c>
+      <c r="C19">
+        <v>883.39</v>
+      </c>
+      <c r="D19">
+        <v>5446.74</v>
+      </c>
+      <c r="E19">
+        <v>-9.19</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>18.1</v>
+      </c>
+      <c r="H19">
+        <v>204.5</v>
+      </c>
+      <c r="I19">
+        <v>312576</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>229373</v>
+      </c>
+      <c r="C20">
+        <v>653.77</v>
+      </c>
+      <c r="D20">
+        <v>3231.97</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>13.98</v>
+      </c>
+      <c r="G20">
+        <v>54.79</v>
+      </c>
+      <c r="H20">
+        <v>244.71</v>
+      </c>
+      <c r="I20">
+        <v>131246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>265359</v>
+      </c>
+      <c r="C21">
+        <v>641.3</v>
+      </c>
+      <c r="D21">
+        <v>3160.38</v>
+      </c>
+      <c r="E21">
+        <v>-3038.25</v>
+      </c>
+      <c r="F21">
+        <v>14.96</v>
+      </c>
+      <c r="G21">
+        <v>66.73</v>
+      </c>
+      <c r="H21">
+        <v>289.94</v>
+      </c>
+      <c r="I21">
+        <v>130377</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>240769</v>
+      </c>
+      <c r="C22">
+        <v>147.53</v>
+      </c>
+      <c r="D22">
+        <v>1178.04</v>
+      </c>
+      <c r="E22">
+        <v>-705</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>12.33</v>
+      </c>
+      <c r="I22">
+        <v>64381</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>299367</v>
+      </c>
+      <c r="C23">
+        <v>34.16</v>
+      </c>
+      <c r="D23">
+        <v>917.49</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>6.38</v>
+      </c>
+      <c r="G23">
+        <v>15.65</v>
+      </c>
+      <c r="H23">
+        <v>30.49</v>
+      </c>
+      <c r="I23">
+        <v>133400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>300806</v>
+      </c>
+      <c r="C24">
+        <v>0.01</v>
+      </c>
+      <c r="D24">
+        <v>0.29</v>
+      </c>
+      <c r="E24">
+        <v>-2.31</v>
+      </c>
+      <c r="F24">
+        <v>-0.11</v>
+      </c>
+      <c r="G24">
+        <v>-0</v>
+      </c>
+      <c r="H24">
+        <v>0.12</v>
+      </c>
+      <c r="I24">
+        <v>18.31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>300806</v>
+      </c>
+      <c r="C25">
+        <v>11598.83</v>
+      </c>
+      <c r="D25">
+        <v>10472.1</v>
+      </c>
+      <c r="E25">
+        <v>1185</v>
+      </c>
+      <c r="F25">
+        <v>5048</v>
+      </c>
+      <c r="G25">
+        <v>9227</v>
+      </c>
+      <c r="H25">
+        <v>14912</v>
+      </c>
+      <c r="I25">
+        <v>722159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>300806</v>
+      </c>
+      <c r="C26">
+        <v>1664.09</v>
+      </c>
+      <c r="D26">
+        <v>781.49</v>
+      </c>
+      <c r="E26">
+        <v>215</v>
+      </c>
+      <c r="F26">
+        <v>1126</v>
+      </c>
+      <c r="G26">
+        <v>1567</v>
+      </c>
+      <c r="H26">
+        <v>2035</v>
+      </c>
+      <c r="I26">
+        <v>14819</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <v>300806</v>
+      </c>
+      <c r="C27">
+        <v>191.39</v>
+      </c>
+      <c r="D27">
+        <v>236.39</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>53</v>
+      </c>
+      <c r="G27">
+        <v>116</v>
+      </c>
+      <c r="H27">
+        <v>237</v>
+      </c>
+      <c r="I27">
+        <v>9603</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>300806</v>
+      </c>
+      <c r="C28">
+        <v>70.29000000000001</v>
+      </c>
+      <c r="D28">
+        <v>74.98</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>23</v>
+      </c>
+      <c r="G28">
+        <v>50</v>
+      </c>
+      <c r="H28">
+        <v>90</v>
+      </c>
+      <c r="I28">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>300806</v>
+      </c>
+      <c r="C29">
+        <v>158.1</v>
+      </c>
+      <c r="D29">
+        <v>160.94</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>55</v>
+      </c>
+      <c r="G29">
+        <v>114</v>
+      </c>
+      <c r="H29">
+        <v>200</v>
+      </c>
+      <c r="I29">
+        <v>4248</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>300806</v>
+      </c>
+      <c r="C30">
+        <v>139.15</v>
+      </c>
+      <c r="D30">
+        <v>309.6</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>30</v>
+      </c>
+      <c r="G30">
+        <v>68</v>
+      </c>
+      <c r="H30">
+        <v>141</v>
+      </c>
+      <c r="I30">
+        <v>27913</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>300806</v>
+      </c>
+      <c r="C31">
+        <v>81.61</v>
+      </c>
+      <c r="D31">
+        <v>100.76</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>24</v>
+      </c>
+      <c r="G31">
+        <v>56</v>
+      </c>
+      <c r="H31">
+        <v>105</v>
+      </c>
+      <c r="I31">
+        <v>7103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>300806</v>
+      </c>
+      <c r="C32">
+        <v>32.6</v>
+      </c>
+      <c r="D32">
+        <v>36.27</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>11</v>
+      </c>
+      <c r="G32">
+        <v>23</v>
+      </c>
+      <c r="H32">
+        <v>42</v>
+      </c>
+      <c r="I32">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
+        <v>300806</v>
+      </c>
+      <c r="C33">
+        <v>36.1</v>
+      </c>
+      <c r="D33">
+        <v>34.6</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>12</v>
+      </c>
+      <c r="G33">
+        <v>27</v>
+      </c>
+      <c r="H33">
+        <v>48</v>
+      </c>
+      <c r="I33">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34">
+        <v>300806</v>
+      </c>
+      <c r="C34">
+        <v>64.06</v>
+      </c>
+      <c r="D34">
+        <v>98.73999999999999</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>15</v>
+      </c>
+      <c r="G34">
+        <v>32</v>
+      </c>
+      <c r="H34">
+        <v>65</v>
+      </c>
+      <c r="I34">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35">
+        <v>300806</v>
+      </c>
+      <c r="C35">
+        <v>4.49</v>
+      </c>
+      <c r="D35">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36">
+        <v>300806</v>
+      </c>
+      <c r="C36">
         <v>-0.01</v>
       </c>
-      <c r="D13">
+      <c r="D36">
         <v>0.01</v>
       </c>
-      <c r="E13">
-        <v>-0.07000000000000001</v>
-      </c>
-      <c r="F13">
+      <c r="E36">
+        <v>-0.06</v>
+      </c>
+      <c r="F36">
         <v>-0.01</v>
       </c>
-      <c r="G13">
+      <c r="G36">
         <v>-0.01</v>
       </c>
-      <c r="H13">
+      <c r="H36">
         <v>-0</v>
       </c>
-      <c r="I13">
-        <v>0.05</v>
+      <c r="I36">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#7 add controls: SIZE, MTB, LEV; variable creation and data screening
</commit_message>
<xml_diff>
--- a/output/Tables.xlsx
+++ b/output/Tables.xlsx
@@ -1672,7 +1672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1729,25 +1729,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>228135</v>
+        <v>202882</v>
       </c>
       <c r="C2" t="n">
-        <v>933.17</v>
+        <v>994.17</v>
       </c>
       <c r="D2" t="n">
-        <v>4139.53</v>
+        <v>4316.58</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>38.01</v>
+        <v>42.97</v>
       </c>
       <c r="G2" t="n">
-        <v>129.88</v>
+        <v>141.5</v>
       </c>
       <c r="H2" t="n">
-        <v>465.03</v>
+        <v>499.68</v>
       </c>
       <c r="I2" t="n">
         <v>167633</v>
@@ -1760,28 +1760,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>299687</v>
+        <v>253295</v>
       </c>
       <c r="C3" t="n">
-        <v>6658.01</v>
+        <v>7021.52</v>
       </c>
       <c r="D3" t="n">
-        <v>59052.73</v>
+        <v>61050.65</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>107.28</v>
+        <v>112.55</v>
       </c>
       <c r="G3" t="n">
-        <v>474.47</v>
+        <v>475.07</v>
       </c>
       <c r="H3" t="n">
-        <v>1961.14</v>
+        <v>1952.41</v>
       </c>
       <c r="I3" t="n">
-        <v>3293755</v>
+        <v>2764661</v>
       </c>
     </row>
     <row r="4">
@@ -1791,25 +1791,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>299140</v>
+        <v>253295</v>
       </c>
       <c r="C4" t="n">
-        <v>1331.75</v>
+        <v>1450.06</v>
       </c>
       <c r="D4" t="n">
-        <v>7503.48</v>
+        <v>7986.68</v>
       </c>
       <c r="E4" t="n">
-        <v>-106362</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>41.65</v>
+        <v>50.45</v>
       </c>
       <c r="G4" t="n">
-        <v>149.62</v>
+        <v>161.43</v>
       </c>
       <c r="H4" t="n">
-        <v>589.89</v>
+        <v>613.34</v>
       </c>
       <c r="I4" t="n">
         <v>397609</v>
@@ -1822,25 +1822,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>299498</v>
+        <v>253212</v>
       </c>
       <c r="C5" t="n">
-        <v>752.67</v>
+        <v>818.7</v>
       </c>
       <c r="D5" t="n">
-        <v>10581.1</v>
+        <v>11245.56</v>
       </c>
       <c r="E5" t="n">
         <v>-26</v>
       </c>
       <c r="F5" t="n">
-        <v>8.699999999999999</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>37.27</v>
+        <v>40.22</v>
       </c>
       <c r="H5" t="n">
-        <v>141.88</v>
+        <v>148.17</v>
       </c>
       <c r="I5" t="n">
         <v>748548</v>
@@ -1853,25 +1853,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>299502</v>
+        <v>253295</v>
       </c>
       <c r="C6" t="n">
-        <v>94.62</v>
+        <v>97.2</v>
       </c>
       <c r="D6" t="n">
-        <v>386.67</v>
+        <v>405.31</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>10.94</v>
+        <v>10.45</v>
       </c>
       <c r="G6" t="n">
-        <v>26.42</v>
+        <v>25.4</v>
       </c>
       <c r="H6" t="n">
-        <v>63.32</v>
+        <v>61.64</v>
       </c>
       <c r="I6" t="n">
         <v>29206.44</v>
@@ -1884,13 +1884,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>274034</v>
+        <v>253295</v>
       </c>
       <c r="C7" t="n">
-        <v>643.17</v>
+        <v>674.67</v>
       </c>
       <c r="D7" t="n">
-        <v>10483.64</v>
+        <v>10687.73</v>
       </c>
       <c r="E7" t="n">
         <v>-0.09</v>
@@ -1899,10 +1899,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2.81</v>
+        <v>2.86</v>
       </c>
       <c r="H7" t="n">
-        <v>30.65</v>
+        <v>32.85</v>
       </c>
       <c r="I7" t="n">
         <v>519230</v>
@@ -1915,28 +1915,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>297205</v>
+        <v>253295</v>
       </c>
       <c r="C8" t="n">
-        <v>1264.37</v>
+        <v>1197.97</v>
       </c>
       <c r="D8" t="n">
-        <v>13910.54</v>
+        <v>9904.440000000001</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="G8" t="n">
-        <v>46.25</v>
+        <v>36.8</v>
       </c>
       <c r="H8" t="n">
-        <v>393.1</v>
+        <v>334.48</v>
       </c>
       <c r="I8" t="n">
-        <v>3048499</v>
+        <v>616814</v>
       </c>
     </row>
     <row r="9">
@@ -1946,25 +1946,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>267133</v>
+        <v>232652</v>
       </c>
       <c r="C9" t="n">
-        <v>30.54</v>
+        <v>32.34</v>
       </c>
       <c r="D9" t="n">
-        <v>168.87</v>
+        <v>174.13</v>
       </c>
       <c r="E9" t="n">
         <v>-33</v>
       </c>
       <c r="F9" t="n">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="G9" t="n">
-        <v>2.26</v>
+        <v>2.43</v>
       </c>
       <c r="H9" t="n">
-        <v>11.77</v>
+        <v>12.52</v>
       </c>
       <c r="I9" t="n">
         <v>8166</v>
@@ -1977,25 +1977,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>299584</v>
+        <v>252950</v>
       </c>
       <c r="C10" t="n">
-        <v>40.99</v>
+        <v>45.85</v>
       </c>
       <c r="D10" t="n">
-        <v>362.35</v>
+        <v>368.69</v>
       </c>
       <c r="E10" t="n">
         <v>-41847.9</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.79</v>
+        <v>-0.4</v>
       </c>
       <c r="G10" t="n">
-        <v>2.1</v>
+        <v>2.29</v>
       </c>
       <c r="H10" t="n">
-        <v>14.72</v>
+        <v>15.28</v>
       </c>
       <c r="I10" t="n">
         <v>22628</v>
@@ -2008,13 +2008,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>212759</v>
+        <v>180278</v>
       </c>
       <c r="C11" t="n">
-        <v>883.39</v>
+        <v>992.09</v>
       </c>
       <c r="D11" t="n">
-        <v>5446.74</v>
+        <v>5868.83</v>
       </c>
       <c r="E11" t="n">
         <v>-9.19</v>
@@ -2023,10 +2023,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>18.1</v>
+        <v>22.01</v>
       </c>
       <c r="H11" t="n">
-        <v>204.5</v>
+        <v>238.44</v>
       </c>
       <c r="I11" t="n">
         <v>312576</v>
@@ -2039,25 +2039,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>229373</v>
+        <v>204118</v>
       </c>
       <c r="C12" t="n">
-        <v>653.77</v>
+        <v>693.41</v>
       </c>
       <c r="D12" t="n">
-        <v>3231.97</v>
+        <v>3366.15</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>13.98</v>
+        <v>14.89</v>
       </c>
       <c r="G12" t="n">
-        <v>54.79</v>
+        <v>58.12</v>
       </c>
       <c r="H12" t="n">
-        <v>244.71</v>
+        <v>260.72</v>
       </c>
       <c r="I12" t="n">
         <v>131246</v>
@@ -2070,25 +2070,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>265359</v>
+        <v>219608</v>
       </c>
       <c r="C13" t="n">
-        <v>641.3</v>
+        <v>702.02</v>
       </c>
       <c r="D13" t="n">
-        <v>3160.38</v>
+        <v>3366.38</v>
       </c>
       <c r="E13" t="n">
         <v>-3038.25</v>
       </c>
       <c r="F13" t="n">
-        <v>14.96</v>
+        <v>16.42</v>
       </c>
       <c r="G13" t="n">
-        <v>66.73</v>
+        <v>72.55</v>
       </c>
       <c r="H13" t="n">
-        <v>289.94</v>
+        <v>323.45</v>
       </c>
       <c r="I13" t="n">
         <v>130377</v>
@@ -2101,13 +2101,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>240769</v>
+        <v>199487</v>
       </c>
       <c r="C14" t="n">
-        <v>147.53</v>
+        <v>170.01</v>
       </c>
       <c r="D14" t="n">
-        <v>1178.04</v>
+        <v>1283.17</v>
       </c>
       <c r="E14" t="n">
         <v>-705</v>
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>12.33</v>
+        <v>16.92</v>
       </c>
       <c r="I14" t="n">
         <v>64381</v>
@@ -2132,28 +2132,28 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>299367</v>
+        <v>253295</v>
       </c>
       <c r="C15" t="n">
-        <v>34.16</v>
+        <v>32.32</v>
       </c>
       <c r="D15" t="n">
-        <v>917.49</v>
+        <v>778.63</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>6.38</v>
+        <v>7.14</v>
       </c>
       <c r="G15" t="n">
-        <v>15.65</v>
+        <v>16.4</v>
       </c>
       <c r="H15" t="n">
-        <v>30.49</v>
+        <v>31.38</v>
       </c>
       <c r="I15" t="n">
-        <v>133400</v>
+        <v>118510</v>
       </c>
     </row>
     <row r="16">
@@ -2163,22 +2163,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D16" t="n">
-        <v>0.29</v>
+        <v>0.28</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.31</v>
+        <v>-1.58</v>
       </c>
       <c r="F16" t="n">
         <v>-0.11</v>
       </c>
       <c r="G16" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>0.12</v>
@@ -2190,29 +2190,29 @@
     <row r="17">
       <c r="A17" s="9" t="inlineStr">
         <is>
-          <t>nw</t>
+          <t>NW</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C17" t="n">
-        <v>11598.83</v>
+        <v>11363.02</v>
       </c>
       <c r="D17" t="n">
-        <v>10472.1</v>
+        <v>10213.56</v>
       </c>
       <c r="E17" t="n">
         <v>1185</v>
       </c>
       <c r="F17" t="n">
-        <v>5048</v>
+        <v>4913</v>
       </c>
       <c r="G17" t="n">
-        <v>9227</v>
+        <v>9010</v>
       </c>
       <c r="H17" t="n">
-        <v>14912</v>
+        <v>14630</v>
       </c>
       <c r="I17" t="n">
         <v>722159</v>
@@ -2225,28 +2225,28 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C18" t="n">
-        <v>1664.09</v>
+        <v>1649.79</v>
       </c>
       <c r="D18" t="n">
-        <v>781.49</v>
+        <v>775.9</v>
       </c>
       <c r="E18" t="n">
         <v>215</v>
       </c>
       <c r="F18" t="n">
-        <v>1126</v>
+        <v>1111</v>
       </c>
       <c r="G18" t="n">
-        <v>1567</v>
+        <v>1552</v>
       </c>
       <c r="H18" t="n">
-        <v>2035</v>
+        <v>2023</v>
       </c>
       <c r="I18" t="n">
-        <v>14819</v>
+        <v>13330</v>
       </c>
     </row>
     <row r="19">
@@ -2256,25 +2256,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C19" t="n">
-        <v>191.39</v>
+        <v>188.2</v>
       </c>
       <c r="D19" t="n">
-        <v>236.39</v>
+        <v>232.94</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H19" t="n">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I19" t="n">
         <v>9603</v>
@@ -2287,13 +2287,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C20" t="n">
-        <v>70.29000000000001</v>
+        <v>69.29000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>74.98</v>
+        <v>74.20999999999999</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -2302,10 +2302,10 @@
         <v>23</v>
       </c>
       <c r="G20" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I20" t="n">
         <v>2828</v>
@@ -2318,25 +2318,25 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C21" t="n">
-        <v>158.1</v>
+        <v>156.3</v>
       </c>
       <c r="D21" t="n">
-        <v>160.94</v>
+        <v>161.19</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G21" t="n">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H21" t="n">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I21" t="n">
         <v>4248</v>
@@ -2349,25 +2349,25 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C22" t="n">
-        <v>139.15</v>
+        <v>135.88</v>
       </c>
       <c r="D22" t="n">
-        <v>309.6</v>
+        <v>296.98</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H22" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I22" t="n">
         <v>27913</v>
@@ -2380,25 +2380,25 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C23" t="n">
-        <v>81.61</v>
+        <v>79.69</v>
       </c>
       <c r="D23" t="n">
-        <v>100.76</v>
+        <v>98.58</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H23" t="n">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I23" t="n">
         <v>7103</v>
@@ -2411,25 +2411,25 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C24" t="n">
-        <v>32.6</v>
+        <v>31.62</v>
       </c>
       <c r="D24" t="n">
-        <v>36.27</v>
+        <v>35.44</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H24" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I24" t="n">
         <v>1804</v>
@@ -2442,13 +2442,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C25" t="n">
-        <v>36.1</v>
+        <v>35.46</v>
       </c>
       <c r="D25" t="n">
-        <v>34.6</v>
+        <v>34.25</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -2457,10 +2457,10 @@
         <v>12</v>
       </c>
       <c r="G25" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I25" t="n">
         <v>992</v>
@@ -2473,25 +2473,25 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C26" t="n">
-        <v>64.06</v>
+        <v>63.18</v>
       </c>
       <c r="D26" t="n">
-        <v>98.73999999999999</v>
+        <v>98.63</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H26" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I26" t="n">
         <v>3190</v>
@@ -2504,13 +2504,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C27" t="n">
-        <v>4.49</v>
+        <v>4.37</v>
       </c>
       <c r="D27" t="n">
-        <v>9.859999999999999</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -2531,11 +2531,11 @@
     <row r="28">
       <c r="A28" s="9" t="inlineStr">
         <is>
-          <t>tone</t>
+          <t>TONE</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>300806</v>
+        <v>253295</v>
       </c>
       <c r="C28" t="n">
         <v>-0.01</v>
@@ -2557,6 +2557,161 @@
       </c>
       <c r="I28" t="n">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9" t="inlineStr">
+        <is>
+          <t>TLAG</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>253295</v>
+      </c>
+      <c r="C29" t="n">
+        <v>40.29</v>
+      </c>
+      <c r="D29" t="n">
+        <v>17.48</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>37</v>
+      </c>
+      <c r="G29" t="n">
+        <v>40</v>
+      </c>
+      <c r="H29" t="n">
+        <v>44</v>
+      </c>
+      <c r="I29" t="n">
+        <v>4072</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="9" t="inlineStr">
+        <is>
+          <t>NEG</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>253295</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="9" t="inlineStr">
+        <is>
+          <t>SIZE</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>253295</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="I31" t="n">
+        <v>11.14</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="9" t="inlineStr">
+        <is>
+          <t>MTB</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>253295</v>
+      </c>
+      <c r="C32" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="I32" t="n">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="9" t="inlineStr">
+        <is>
+          <t>LEV</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>253295</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify TLAG def; 8-K data merge WIP
</commit_message>
<xml_diff>
--- a/output/Tables.xlsx
+++ b/output/Tables.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="T1PA_raw" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -87,7 +87,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -111,6 +111,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -449,20 +450,20 @@
   </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col width="19.21875" customWidth="1" min="1" max="1"/>
-    <col width="9.21875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="9" bestFit="1" customWidth="1" min="6" max="8"/>
-    <col width="9.5546875" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="39.6640625" customWidth="1" min="11" max="11"/>
+    <col width="19.21875" customWidth="1" style="9" min="1" max="1"/>
+    <col width="9.21875" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="9" bestFit="1" customWidth="1" style="9" min="6" max="8"/>
+    <col width="9.5546875" bestFit="1" customWidth="1" style="9" min="9" max="9"/>
+    <col width="39.6640625" customWidth="1" style="9" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" s="9">
       <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Preliminary Summary Statistics</t>
@@ -1672,7 +1673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1681,1037 +1682,417 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>count</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>mean</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>std</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>min</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>25%</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>50%</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>75%</t>
         </is>
       </c>
-      <c r="I1" s="9" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>max</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="inlineStr">
-        <is>
-          <t>actq</t>
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>NW</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>202882</v>
+        <v>189501</v>
       </c>
       <c r="C2" t="n">
-        <v>994.17</v>
+        <v>10935.16</v>
       </c>
       <c r="D2" t="n">
-        <v>4316.58</v>
+        <v>10059.14</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1157</v>
       </c>
       <c r="F2" t="n">
-        <v>42.97</v>
+        <v>4734</v>
       </c>
       <c r="G2" t="n">
-        <v>141.5</v>
+        <v>8700</v>
       </c>
       <c r="H2" t="n">
-        <v>499.68</v>
+        <v>13933</v>
       </c>
       <c r="I2" t="n">
-        <v>167633</v>
+        <v>722159</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>atq</t>
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>TONE</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>253295</v>
+        <v>189501</v>
       </c>
       <c r="C3" t="n">
-        <v>7021.52</v>
+        <v>-0.01</v>
       </c>
       <c r="D3" t="n">
-        <v>61050.65</v>
+        <v>0.01</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-0.06</v>
       </c>
       <c r="F3" t="n">
-        <v>112.55</v>
+        <v>-0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>475.07</v>
+        <v>-0.01</v>
       </c>
       <c r="H3" t="n">
-        <v>1952.41</v>
+        <v>-0</v>
       </c>
       <c r="I3" t="n">
-        <v>2764661</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>ceqq</t>
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>TLAG</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>253295</v>
+        <v>189501</v>
       </c>
       <c r="C4" t="n">
-        <v>1450.06</v>
+        <v>39.47</v>
       </c>
       <c r="D4" t="n">
-        <v>7986.68</v>
+        <v>6.19</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>50.45</v>
+        <v>36</v>
       </c>
       <c r="G4" t="n">
-        <v>161.43</v>
+        <v>40</v>
       </c>
       <c r="H4" t="n">
-        <v>613.34</v>
+        <v>45</v>
       </c>
       <c r="I4" t="n">
-        <v>397609</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>cheq</t>
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>n_neg</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>253212</v>
+        <v>189501</v>
       </c>
       <c r="C5" t="n">
-        <v>818.7</v>
+        <v>183.59</v>
       </c>
       <c r="D5" t="n">
-        <v>11245.56</v>
+        <v>236.66</v>
       </c>
       <c r="E5" t="n">
-        <v>-26</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>9.710000000000001</v>
+        <v>48</v>
       </c>
       <c r="G5" t="n">
-        <v>40.22</v>
+        <v>108</v>
       </c>
       <c r="H5" t="n">
-        <v>148.17</v>
+        <v>218</v>
       </c>
       <c r="I5" t="n">
-        <v>748548</v>
+        <v>9603</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>cshoq</t>
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>n_pos</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>253295</v>
+        <v>189501</v>
       </c>
       <c r="C6" t="n">
-        <v>97.2</v>
+        <v>69.39</v>
       </c>
       <c r="D6" t="n">
-        <v>405.31</v>
+        <v>76.53</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>10.45</v>
+        <v>22</v>
       </c>
       <c r="G6" t="n">
-        <v>25.4</v>
+        <v>48</v>
       </c>
       <c r="H6" t="n">
-        <v>61.64</v>
+        <v>88</v>
       </c>
       <c r="I6" t="n">
-        <v>29206.44</v>
+        <v>2828</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>dlcq</t>
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>n_negation</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>253295</v>
+        <v>189501</v>
       </c>
       <c r="C7" t="n">
-        <v>674.67</v>
+        <v>4.84</v>
       </c>
       <c r="D7" t="n">
-        <v>10687.73</v>
+        <v>10.21</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.09</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2.86</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>32.85</v>
+        <v>5</v>
       </c>
       <c r="I7" t="n">
-        <v>519230</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>dlttq</t>
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>nvocab</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>253295</v>
+        <v>189501</v>
       </c>
       <c r="C8" t="n">
-        <v>1197.97</v>
+        <v>1627.64</v>
       </c>
       <c r="D8" t="n">
-        <v>9904.440000000001</v>
+        <v>783.22</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="F8" t="n">
-        <v>0.22</v>
+        <v>1088</v>
       </c>
       <c r="G8" t="n">
-        <v>36.8</v>
+        <v>1523</v>
       </c>
       <c r="H8" t="n">
-        <v>334.48</v>
+        <v>1991</v>
       </c>
       <c r="I8" t="n">
-        <v>616814</v>
+        <v>13330</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="inlineStr">
-        <is>
-          <t>dpq</t>
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>RET</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>232652</v>
+        <v>189501</v>
       </c>
       <c r="C9" t="n">
-        <v>32.34</v>
+        <v>0.02</v>
       </c>
       <c r="D9" t="n">
-        <v>174.13</v>
+        <v>0.3</v>
       </c>
       <c r="E9" t="n">
-        <v>-33</v>
+        <v>-1.58</v>
       </c>
       <c r="F9" t="n">
-        <v>0.52</v>
+        <v>-0.13</v>
       </c>
       <c r="G9" t="n">
-        <v>2.43</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>12.52</v>
+        <v>0.13</v>
       </c>
       <c r="I9" t="n">
-        <v>8166</v>
+        <v>18.31</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="inlineStr">
-        <is>
-          <t>ibq</t>
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>NEG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>252950</v>
+        <v>189501</v>
       </c>
       <c r="C10" t="n">
-        <v>45.85</v>
+        <v>0.5</v>
       </c>
       <c r="D10" t="n">
-        <v>368.69</v>
+        <v>0.5</v>
       </c>
       <c r="E10" t="n">
-        <v>-41847.9</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>2.29</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>15.28</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>22628</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="inlineStr">
-        <is>
-          <t>intanq</t>
+      <c r="A11" s="10" t="inlineStr">
+        <is>
+          <t>SIZE</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>180278</v>
+        <v>189501</v>
       </c>
       <c r="C11" t="n">
-        <v>992.09</v>
+        <v>6.02</v>
       </c>
       <c r="D11" t="n">
-        <v>5868.83</v>
+        <v>1.99</v>
       </c>
       <c r="E11" t="n">
-        <v>-9.19</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>4.55</v>
       </c>
       <c r="G11" t="n">
-        <v>22.01</v>
+        <v>5.91</v>
       </c>
       <c r="H11" t="n">
-        <v>238.44</v>
+        <v>7.32</v>
       </c>
       <c r="I11" t="n">
-        <v>312576</v>
+        <v>11.23</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="inlineStr">
-        <is>
-          <t>lctq</t>
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>MTB</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>204118</v>
+        <v>189501</v>
       </c>
       <c r="C12" t="n">
-        <v>693.41</v>
+        <v>3.78</v>
       </c>
       <c r="D12" t="n">
-        <v>3366.15</v>
+        <v>5.05</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="F12" t="n">
-        <v>14.89</v>
+        <v>1.36</v>
       </c>
       <c r="G12" t="n">
-        <v>58.12</v>
+        <v>2.26</v>
       </c>
       <c r="H12" t="n">
-        <v>260.72</v>
+        <v>4.01</v>
       </c>
       <c r="I12" t="n">
-        <v>131246</v>
+        <v>35.88</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="inlineStr">
-        <is>
-          <t>revtq</t>
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>LEV</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>219608</v>
+        <v>189501</v>
       </c>
       <c r="C13" t="n">
-        <v>702.02</v>
+        <v>0.2</v>
       </c>
       <c r="D13" t="n">
-        <v>3366.38</v>
+        <v>0.19</v>
       </c>
       <c r="E13" t="n">
-        <v>-3038.25</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>16.42</v>
+        <v>0.01</v>
       </c>
       <c r="G13" t="n">
-        <v>72.55</v>
+        <v>0.17</v>
       </c>
       <c r="H13" t="n">
-        <v>323.45</v>
+        <v>0.33</v>
       </c>
       <c r="I13" t="n">
-        <v>130377</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="9" t="inlineStr">
-        <is>
-          <t>txditcq</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>199487</v>
-      </c>
-      <c r="C14" t="n">
-        <v>170.01</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1283.17</v>
-      </c>
-      <c r="E14" t="n">
-        <v>-705</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>16.92</v>
-      </c>
-      <c r="I14" t="n">
-        <v>64381</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="9" t="inlineStr">
-        <is>
-          <t>prccq</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C15" t="n">
-        <v>32.32</v>
-      </c>
-      <c r="D15" t="n">
-        <v>778.63</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>7.14</v>
-      </c>
-      <c r="G15" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="H15" t="n">
-        <v>31.38</v>
-      </c>
-      <c r="I15" t="n">
-        <v>118510</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="9" t="inlineStr">
-        <is>
-          <t>RET</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="E16" t="n">
-        <v>-1.58</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-0.11</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="I16" t="n">
-        <v>18.31</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="9" t="inlineStr">
-        <is>
-          <t>NW</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C17" t="n">
-        <v>11363.02</v>
-      </c>
-      <c r="D17" t="n">
-        <v>10213.56</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1185</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4913</v>
-      </c>
-      <c r="G17" t="n">
-        <v>9010</v>
-      </c>
-      <c r="H17" t="n">
-        <v>14630</v>
-      </c>
-      <c r="I17" t="n">
-        <v>722159</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="9" t="inlineStr">
-        <is>
-          <t>nvocab</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1649.79</v>
-      </c>
-      <c r="D18" t="n">
-        <v>775.9</v>
-      </c>
-      <c r="E18" t="n">
-        <v>215</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1111</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1552</v>
-      </c>
-      <c r="H18" t="n">
-        <v>2023</v>
-      </c>
-      <c r="I18" t="n">
-        <v>13330</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="inlineStr">
-        <is>
-          <t>n_neg</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C19" t="n">
-        <v>188.2</v>
-      </c>
-      <c r="D19" t="n">
-        <v>232.94</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>51</v>
-      </c>
-      <c r="G19" t="n">
-        <v>114</v>
-      </c>
-      <c r="H19" t="n">
-        <v>234</v>
-      </c>
-      <c r="I19" t="n">
-        <v>9603</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="9" t="inlineStr">
-        <is>
-          <t>n_pos</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C20" t="n">
-        <v>69.29000000000001</v>
-      </c>
-      <c r="D20" t="n">
-        <v>74.20999999999999</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
-        <v>23</v>
-      </c>
-      <c r="G20" t="n">
-        <v>49</v>
-      </c>
-      <c r="H20" t="n">
-        <v>89</v>
-      </c>
-      <c r="I20" t="n">
-        <v>2828</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="inlineStr">
-        <is>
-          <t>n_uctt</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C21" t="n">
-        <v>156.3</v>
-      </c>
-      <c r="D21" t="n">
-        <v>161.19</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>53</v>
-      </c>
-      <c r="G21" t="n">
-        <v>111</v>
-      </c>
-      <c r="H21" t="n">
-        <v>197</v>
-      </c>
-      <c r="I21" t="n">
-        <v>4248</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="inlineStr">
-        <is>
-          <t>n_lit</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C22" t="n">
-        <v>135.88</v>
-      </c>
-      <c r="D22" t="n">
-        <v>296.98</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>29</v>
-      </c>
-      <c r="G22" t="n">
-        <v>67</v>
-      </c>
-      <c r="H22" t="n">
-        <v>140</v>
-      </c>
-      <c r="I22" t="n">
-        <v>27913</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="9" t="inlineStr">
-        <is>
-          <t>n_cstr</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C23" t="n">
-        <v>79.69</v>
-      </c>
-      <c r="D23" t="n">
-        <v>98.58</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
-        <v>23</v>
-      </c>
-      <c r="G23" t="n">
-        <v>54</v>
-      </c>
-      <c r="H23" t="n">
-        <v>102</v>
-      </c>
-      <c r="I23" t="n">
-        <v>7103</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="9" t="inlineStr">
-        <is>
-          <t>n_modal_strong</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C24" t="n">
-        <v>31.62</v>
-      </c>
-      <c r="D24" t="n">
-        <v>35.44</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>10</v>
-      </c>
-      <c r="G24" t="n">
-        <v>22</v>
-      </c>
-      <c r="H24" t="n">
-        <v>41</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1804</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="9" t="inlineStr">
-        <is>
-          <t>n_modal_moderate</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C25" t="n">
-        <v>35.46</v>
-      </c>
-      <c r="D25" t="n">
-        <v>34.25</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>12</v>
-      </c>
-      <c r="G25" t="n">
-        <v>26</v>
-      </c>
-      <c r="H25" t="n">
-        <v>47</v>
-      </c>
-      <c r="I25" t="n">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="9" t="inlineStr">
-        <is>
-          <t>n_modal_weak</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C26" t="n">
-        <v>63.18</v>
-      </c>
-      <c r="D26" t="n">
-        <v>98.63</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>14</v>
-      </c>
-      <c r="G26" t="n">
-        <v>31</v>
-      </c>
-      <c r="H26" t="n">
-        <v>64</v>
-      </c>
-      <c r="I26" t="n">
-        <v>3190</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="9" t="inlineStr">
-        <is>
-          <t>n_negation</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C27" t="n">
-        <v>4.37</v>
-      </c>
-      <c r="D27" t="n">
-        <v>9.800000000000001</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" t="n">
-        <v>4</v>
-      </c>
-      <c r="I27" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="9" t="inlineStr">
-        <is>
-          <t>TONE</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C28" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E28" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="F28" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="G28" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="H28" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="9" t="inlineStr">
-        <is>
-          <t>TLAG</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C29" t="n">
-        <v>40.29</v>
-      </c>
-      <c r="D29" t="n">
-        <v>17.48</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
-        <v>37</v>
-      </c>
-      <c r="G29" t="n">
-        <v>40</v>
-      </c>
-      <c r="H29" t="n">
-        <v>44</v>
-      </c>
-      <c r="I29" t="n">
-        <v>4072</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="9" t="inlineStr">
-        <is>
-          <t>NEG</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" t="n">
-        <v>1</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="9" t="inlineStr">
-        <is>
-          <t>SIZE</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C31" t="n">
-        <v>5.99</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="E31" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="F31" t="n">
-        <v>4.52</v>
-      </c>
-      <c r="G31" t="n">
-        <v>5.86</v>
-      </c>
-      <c r="H31" t="n">
-        <v>7.3</v>
-      </c>
-      <c r="I31" t="n">
-        <v>11.14</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="9" t="inlineStr">
-        <is>
-          <t>MTB</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C32" t="n">
-        <v>3.38</v>
-      </c>
-      <c r="D32" t="n">
-        <v>4.74</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="F32" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="G32" t="n">
-        <v>1.96</v>
-      </c>
-      <c r="H32" t="n">
-        <v>3.49</v>
-      </c>
-      <c r="I32" t="n">
-        <v>34.56</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="9" t="inlineStr">
-        <is>
-          <t>LEV</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>253295</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0.77</v>
+        <v>0.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create T1PB: correlation matrix and T2: results_10-Q
</commit_message>
<xml_diff>
--- a/output/Tables.xlsx
+++ b/output/Tables.xlsx
@@ -8,23 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\narrative_conservatism\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224BEC6E-F321-4072-B96C-644A99E4952F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7116B933-345A-4158-9747-0DEE9CB5DD02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T1PA" sheetId="1" r:id="rId1"/>
-    <sheet name="T1PA_raw" sheetId="2" r:id="rId2"/>
+    <sheet name="T1PB" sheetId="2" r:id="rId2"/>
+    <sheet name="T1PA_raw" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="T2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
-  <si>
-    <t>Preliminary Summary Statistics 10-Q</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="201">
   <si>
     <t>count</t>
   </si>
@@ -194,33 +193,54 @@
     <t>NW</t>
   </si>
   <si>
+    <t>natural logarithm of number of total words</t>
+  </si>
+  <si>
+    <t>NW = log(nw)</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>number of total words</t>
+  </si>
+  <si>
+    <t>TONE</t>
+  </si>
+  <si>
+    <t>tone, defined as number of net positive words (n_pos - n_neg - n_negations) per 1000 total words</t>
+  </si>
+  <si>
+    <t>tone = (n_pos - n_negation - n_neg)*1000/nw</t>
+  </si>
+  <si>
+    <t>TLAG</t>
+  </si>
+  <si>
+    <t>number of days between the news release date (CRSP quarter-end date) and document filing date (EDGAR filing date)</t>
+  </si>
+  <si>
+    <t>TLAG = fd - date_crsp</t>
+  </si>
+  <si>
+    <t>nvocab</t>
+  </si>
+  <si>
+    <t>number of total vocabulary</t>
+  </si>
+  <si>
+    <t>n_neg</t>
+  </si>
+  <si>
+    <t>number of negative words</t>
+  </si>
+  <si>
+    <t>n_pos</t>
+  </si>
+  <si>
     <t>number of positive words</t>
   </si>
   <si>
-    <t>TONE</t>
-  </si>
-  <si>
-    <t>TLAG</t>
-  </si>
-  <si>
-    <t>number of days between the news release date (CRSP quarter-end date) and document filing date (EDGAR filing date)</t>
-  </si>
-  <si>
-    <t>nvocab</t>
-  </si>
-  <si>
-    <t>number of total vocabulary</t>
-  </si>
-  <si>
-    <t>n_neg</t>
-  </si>
-  <si>
-    <t>number of negative words</t>
-  </si>
-  <si>
-    <t>n_pos</t>
-  </si>
-  <si>
     <t>n_uctt</t>
   </si>
   <si>
@@ -266,32 +286,356 @@
     <t>Note: word counts are based on LM dictionary</t>
   </si>
   <si>
-    <t>nw</t>
-  </si>
-  <si>
-    <t>tone, defined as number of net positive words (n_pos - n_neg - n_negations) per 1000 total words</t>
-  </si>
-  <si>
-    <t>NW = log(nw)</t>
-  </si>
-  <si>
-    <t>tone = (n_pos - n_negation - n_neg)*1000/nw</t>
-  </si>
-  <si>
-    <t>TLAG = fd - date_crsp</t>
-  </si>
-  <si>
-    <t>number of total words</t>
-  </si>
-  <si>
-    <t>natural logarithm of number of total words</t>
+    <t>(1)</t>
+  </si>
+  <si>
+    <t>(2)</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>(4)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>VARIABLES</t>
+  </si>
+  <si>
+    <t>0.114***</t>
+  </si>
+  <si>
+    <t>0.032***</t>
+  </si>
+  <si>
+    <t>-1.692***</t>
+  </si>
+  <si>
+    <t>-0.469***</t>
+  </si>
+  <si>
+    <t>0.974***</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>(13.430)</t>
+  </si>
+  <si>
+    <t>(4.343)</t>
+  </si>
+  <si>
+    <t>(-21.815)</t>
+  </si>
+  <si>
+    <t>(-5.996)</t>
+  </si>
+  <si>
+    <t>(4.706)</t>
+  </si>
+  <si>
+    <t>(0.011)</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>-0.001</t>
+  </si>
+  <si>
+    <t>0.275***</t>
+  </si>
+  <si>
+    <t>-0.015</t>
+  </si>
+  <si>
+    <t>-0.290***</t>
+  </si>
+  <si>
+    <t>-0.005</t>
+  </si>
+  <si>
+    <t>(0.731)</t>
+  </si>
+  <si>
+    <t>(-0.397)</t>
+  </si>
+  <si>
+    <t>(6.580)</t>
+  </si>
+  <si>
+    <t>(-0.482)</t>
+  </si>
+  <si>
+    <t>(-2.598)</t>
+  </si>
+  <si>
+    <t>(-0.045)</t>
+  </si>
+  <si>
+    <t>RET_NEG</t>
+  </si>
+  <si>
+    <t>-0.631***</t>
+  </si>
+  <si>
+    <t>-0.177***</t>
+  </si>
+  <si>
+    <t>7.588***</t>
+  </si>
+  <si>
+    <t>1.792***</t>
+  </si>
+  <si>
+    <t>-5.855***</t>
+  </si>
+  <si>
+    <t>-2.407***</t>
+  </si>
+  <si>
+    <t>(-36.373)</t>
+  </si>
+  <si>
+    <t>(-12.206)</t>
+  </si>
+  <si>
+    <t>(47.837)</t>
+  </si>
+  <si>
+    <t>(10.428)</t>
+  </si>
+  <si>
+    <t>(-13.828)</t>
+  </si>
+  <si>
+    <t>(-4.484)</t>
+  </si>
+  <si>
+    <t>0.134***</t>
+  </si>
+  <si>
+    <t>0.039***</t>
+  </si>
+  <si>
+    <t>-0.337***</t>
+  </si>
+  <si>
+    <t>0.664***</t>
+  </si>
+  <si>
+    <t>-1.302***</t>
+  </si>
+  <si>
+    <t>-0.649***</t>
+  </si>
+  <si>
+    <t>(148.850)</t>
+  </si>
+  <si>
+    <t>(6.867)</t>
+  </si>
+  <si>
+    <t>(-41.072)</t>
+  </si>
+  <si>
+    <t>(9.609)</t>
+  </si>
+  <si>
+    <t>(-59.371)</t>
+  </si>
+  <si>
+    <t>(-5.698)</t>
+  </si>
+  <si>
+    <t>0.004***</t>
+  </si>
+  <si>
+    <t>-0.004***</t>
+  </si>
+  <si>
+    <t>-0.024***</t>
+  </si>
+  <si>
+    <t>0.028***</t>
+  </si>
+  <si>
+    <t>0.044***</t>
+  </si>
+  <si>
+    <t>-0.009</t>
+  </si>
+  <si>
+    <t>(12.882)</t>
+  </si>
+  <si>
+    <t>(-7.399)</t>
+  </si>
+  <si>
+    <t>(-7.703)</t>
+  </si>
+  <si>
+    <t>(4.091)</t>
+  </si>
+  <si>
+    <t>(5.166)</t>
+  </si>
+  <si>
+    <t>(-0.379)</t>
+  </si>
+  <si>
+    <t>0.139***</t>
+  </si>
+  <si>
+    <t>0.438***</t>
+  </si>
+  <si>
+    <t>2.405***</t>
+  </si>
+  <si>
+    <t>-1.930***</t>
+  </si>
+  <si>
+    <t>1.066***</t>
+  </si>
+  <si>
+    <t>2.613***</t>
+  </si>
+  <si>
+    <t>(15.525)</t>
+  </si>
+  <si>
+    <t>(17.386)</t>
+  </si>
+  <si>
+    <t>(29.294)</t>
+  </si>
+  <si>
+    <t>(-6.301)</t>
+  </si>
+  <si>
+    <t>(4.862)</t>
+  </si>
+  <si>
+    <t>(4.267)</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>8.097***</t>
+  </si>
+  <si>
+    <t>7.616***</t>
+  </si>
+  <si>
+    <t>-6.377***</t>
+  </si>
+  <si>
+    <t>-6.394*</t>
+  </si>
+  <si>
+    <t>47.422***</t>
+  </si>
+  <si>
+    <t>188.543***</t>
+  </si>
+  <si>
+    <t>(1,249.737)</t>
+  </si>
+  <si>
+    <t>(110.391)</t>
+  </si>
+  <si>
+    <t>(-107.680)</t>
+  </si>
+  <si>
+    <t>(-1.657)</t>
+  </si>
+  <si>
+    <t>(299.981)</t>
+  </si>
+  <si>
+    <t>(3.311)</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>190,926</t>
+  </si>
+  <si>
+    <t>R-squared</t>
+  </si>
+  <si>
+    <t>0.118</t>
+  </si>
+  <si>
+    <t>0.695</t>
+  </si>
+  <si>
+    <t>0.022</t>
+  </si>
+  <si>
+    <t>0.568</t>
+  </si>
+  <si>
+    <t>0.023</t>
+  </si>
+  <si>
+    <t>0.149</t>
+  </si>
+  <si>
+    <t>Quarter FE</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Firm FE</t>
+  </si>
+  <si>
+    <t>Industry-clustered SE</t>
+  </si>
+  <si>
+    <t>t-statistics in parentheses</t>
+  </si>
+  <si>
+    <t>*** p&lt;0.01, ** p&lt;0.05, * p&lt;0.1</t>
+  </si>
+  <si>
+    <t>Doc_measure = b0 + b1*RET + b2*NEG + b3*RET*NEG + controls, where doc_measure = NW, TONE, TLAG</t>
+  </si>
+  <si>
+    <t>Table 1. Panel A: Summary Statistics 10-Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: right-up matrix: pearson; left-down matrix: spearman </t>
+  </si>
+  <si>
+    <t>Table 1. Panel B: Correlation Matrix</t>
+  </si>
+  <si>
+    <t>Table 2: Main Results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,20 +671,42 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -393,11 +759,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -415,29 +830,59 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -781,75 +1226,75 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="8.33203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="2.109375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="96.77734375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.33203125" style="21" customWidth="1"/>
+    <col min="10" max="10" width="2.109375" style="21" customWidth="1"/>
+    <col min="11" max="11" width="96.77734375" style="21" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="A1" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="K3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
@@ -860,15 +1305,15 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
         <v>13</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
@@ -879,15 +1324,15 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
@@ -898,15 +1343,15 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
@@ -917,15 +1362,15 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
@@ -936,15 +1381,15 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="K8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
@@ -955,15 +1400,15 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
@@ -974,15 +1419,15 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -993,15 +1438,15 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="K11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -1012,15 +1457,15 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="K12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
@@ -1031,15 +1476,15 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="K13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="3"/>
@@ -1050,15 +1495,15 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="K14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
@@ -1069,15 +1514,15 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="K15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
@@ -1088,15 +1533,15 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="K16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -1107,187 +1552,187 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4">
         <v>190926</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>0.02</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>0.3</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>-1.58</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>-0.13</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>0</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>0.13</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="8">
         <v>18.309999999999999</v>
       </c>
       <c r="K18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" t="s">
         <v>42</v>
-      </c>
-      <c r="L18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4">
         <v>190926</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>0.49934000000000001</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>0.50000100000000003</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>0</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>0</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>1</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4">
         <v>190926</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>6.01</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>1.99</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>1.99</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>4.54</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>5.91</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>7.32</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>11.23</v>
       </c>
       <c r="K20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" t="s">
         <v>47</v>
-      </c>
-      <c r="L20" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4">
         <v>190926</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>3.77</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>5.05</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>0.35</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>1.35</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>2.2599999999999998</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>4</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="8">
         <v>35.82</v>
       </c>
       <c r="K21" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" t="s">
         <v>50</v>
-      </c>
-      <c r="L21" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4">
         <v>190926</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>0.2</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>0.19</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>0</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="8">
         <v>0.01</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <v>0.17</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <v>0.33</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="8">
         <v>0.72</v>
       </c>
       <c r="K22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L22" t="s">
         <v>53</v>
-      </c>
-      <c r="L22" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1298,44 +1743,44 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>56</v>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="B24" s="3">
         <v>190926</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>9</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>0.78</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>7.05</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>8.4700000000000006</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <v>9.07</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <v>9.5399999999999991</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="8">
         <v>13.49</v>
       </c>
-      <c r="K24" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>83</v>
+      <c r="K24" t="s">
+        <v>56</v>
+      </c>
+      <c r="L24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B25" s="4">
         <v>190926</v>
@@ -1362,15 +1807,15 @@
         <v>722159</v>
       </c>
       <c r="K25" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="L25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B26" s="4">
         <v>190926</v>
@@ -1397,15 +1842,15 @@
         <v>22.29</v>
       </c>
       <c r="K26" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="L26" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B27" s="4">
         <v>190926</v>
@@ -1432,15 +1877,15 @@
         <v>4069</v>
       </c>
       <c r="K27" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L27" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B28" s="4">
         <v>190926</v>
@@ -1467,15 +1912,15 @@
         <v>13330</v>
       </c>
       <c r="K28" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B29" s="4">
         <v>190926</v>
@@ -1502,15 +1947,15 @@
         <v>9603</v>
       </c>
       <c r="K29" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B30" s="4">
         <v>190926</v>
@@ -1537,15 +1982,15 @@
         <v>2828</v>
       </c>
       <c r="K30" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="L30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
@@ -1556,15 +2001,15 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="K31" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="L31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
@@ -1575,15 +2020,15 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="K32" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="L32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
@@ -1594,15 +2039,15 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="K33" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="L33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
@@ -1613,15 +2058,15 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="K34" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="L34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
@@ -1632,15 +2077,15 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="K35" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="L35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
@@ -1651,15 +2096,15 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="K36" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="L36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B37" s="4">
         <v>190926</v>
@@ -1686,34 +2131,34 @@
         <v>285</v>
       </c>
       <c r="K37" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="L37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K39" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1726,43 +2171,702 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" style="21" customWidth="1"/>
+    <col min="2" max="14" width="10.88671875" style="21" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="23">
+        <v>1</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="D3" s="23">
+        <v>-0.44700000000000001</v>
+      </c>
+      <c r="E3" s="23">
+        <v>-5.0999999999999997E-2</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="J3" s="23">
+        <v>-1.7999999999999999E-2</v>
+      </c>
+      <c r="K3" s="23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L3" s="23">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="M3" s="23">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="N3" s="23">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="23">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23">
+        <v>1</v>
+      </c>
+      <c r="D4" s="23">
+        <v>-0.378</v>
+      </c>
+      <c r="E4" s="23">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="F4" s="23">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0.498</v>
+      </c>
+      <c r="I4" s="23">
+        <v>0.87</v>
+      </c>
+      <c r="J4" s="23">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="K4" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="L4" s="23">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="M4" s="23">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="N4" s="23">
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="23">
+        <v>-0.45600000000000002</v>
+      </c>
+      <c r="C5" s="23">
+        <v>-0.45600000000000002</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1</v>
+      </c>
+      <c r="E5" s="23">
+        <v>-3.5999999999999997E-2</v>
+      </c>
+      <c r="F5" s="23">
+        <v>-0.60699999999999998</v>
+      </c>
+      <c r="G5" s="23">
+        <v>-0.34899999999999998</v>
+      </c>
+      <c r="H5" s="23">
+        <v>-0.38800000000000001</v>
+      </c>
+      <c r="I5" s="23">
+        <v>-0.46800000000000003</v>
+      </c>
+      <c r="J5" s="23">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K5" s="23">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="L5" s="23">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="M5" s="23">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="N5" s="23">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="23">
+        <v>-0.28299999999999997</v>
+      </c>
+      <c r="C6" s="23">
+        <v>-0.28299999999999997</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E6" s="23">
+        <v>1</v>
+      </c>
+      <c r="F6" s="23">
+        <v>-1E-3</v>
+      </c>
+      <c r="G6" s="23">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="H6" s="23">
+        <v>0</v>
+      </c>
+      <c r="I6" s="23">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="J6" s="23">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K6" s="23">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="L6" s="23">
+        <v>-0.14699999999999999</v>
+      </c>
+      <c r="M6" s="23">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="N6" s="23">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="23">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="D7" s="23">
+        <v>-0.72399999999999998</v>
+      </c>
+      <c r="E7" s="23">
+        <v>-0.22800000000000001</v>
+      </c>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.874</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="I7" s="23">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="J7" s="23">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="K7" s="23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L7" s="23">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="M7" s="23">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="N7" s="23">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="D8" s="23">
+        <v>-0.37</v>
+      </c>
+      <c r="E8" s="23">
+        <v>-0.29899999999999999</v>
+      </c>
+      <c r="F8" s="23">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="G8" s="23">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="J8" s="23">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="K8" s="23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L8" s="23">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="M8" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="N8" s="23">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="23">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="D9" s="23">
+        <v>-0.42199999999999999</v>
+      </c>
+      <c r="E9" s="23">
+        <v>-0.08</v>
+      </c>
+      <c r="F9" s="23">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H9" s="23">
+        <v>1</v>
+      </c>
+      <c r="I9" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="23">
+        <v>-1E-3</v>
+      </c>
+      <c r="K9" s="23">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L9" s="23">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="M9" s="23">
+        <v>0.111</v>
+      </c>
+      <c r="N9" s="23">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="23">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="D10" s="23">
+        <v>-0.501</v>
+      </c>
+      <c r="E10" s="23">
+        <v>-0.216</v>
+      </c>
+      <c r="F10" s="23">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="H10" s="23">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="I10" s="23">
+        <v>1</v>
+      </c>
+      <c r="J10" s="23">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="K10" s="23">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="L10" s="23">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="M10" s="23">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="N10" s="23">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="23">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="C11" s="23">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="D11" s="23">
+        <v>2.7E-2</v>
+      </c>
+      <c r="E11" s="23">
+        <v>-0.04</v>
+      </c>
+      <c r="F11" s="23">
+        <v>-0.02</v>
+      </c>
+      <c r="G11" s="23">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="H11" s="23">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="I11" s="23">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="J11" s="23">
+        <v>1</v>
+      </c>
+      <c r="K11" s="23">
+        <v>-0.63600000000000001</v>
+      </c>
+      <c r="L11" s="23">
+        <v>4.7E-2</v>
+      </c>
+      <c r="M11" s="23">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="N11" s="23">
+        <v>-1.9E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="C12" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="23">
+        <v>-0.02</v>
+      </c>
+      <c r="E12" s="23">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F12" s="23">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G12" s="23">
+        <v>2E-3</v>
+      </c>
+      <c r="H12" s="23">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I12" s="23">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J12" s="23">
+        <v>-0.86599999999999999</v>
+      </c>
+      <c r="K12" s="23">
+        <v>1</v>
+      </c>
+      <c r="L12" s="23">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="M12" s="23">
+        <v>-0.10100000000000001</v>
+      </c>
+      <c r="N12" s="23">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="C13" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="D13" s="23">
+        <v>-5.0999999999999997E-2</v>
+      </c>
+      <c r="E13" s="23">
+        <v>-0.42699999999999999</v>
+      </c>
+      <c r="F13" s="23">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G13" s="23">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="H13" s="23">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0.107</v>
+      </c>
+      <c r="K13" s="23">
+        <v>-0.10100000000000001</v>
+      </c>
+      <c r="L13" s="23">
+        <v>1</v>
+      </c>
+      <c r="M13" s="23">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="N13" s="23">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="C14" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="D14" s="23">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E14" s="23">
+        <v>-0.10199999999999999</v>
+      </c>
+      <c r="F14" s="23">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G14" s="23">
+        <v>0.153</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0.105</v>
+      </c>
+      <c r="I14" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="J14" s="23">
+        <v>0.193</v>
+      </c>
+      <c r="K14" s="23">
+        <v>-0.16200000000000001</v>
+      </c>
+      <c r="L14" s="23">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="M14" s="23">
+        <v>1</v>
+      </c>
+      <c r="N14" s="23">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="23">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C15" s="23">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D15" s="23">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E15" s="23">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="F15" s="23">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G15" s="23">
+        <v>1.4E-2</v>
+      </c>
+      <c r="H15" s="23">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I15" s="23">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J15" s="23">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="K15" s="23">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L15" s="23">
+        <v>0.153</v>
+      </c>
+      <c r="M15" s="23">
+        <v>-5.1999999999999998E-2</v>
+      </c>
+      <c r="N15" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>56</v>
+      <c r="A2" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="B2">
         <v>190926</v>
@@ -1790,8 +2894,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>81</v>
+      <c r="A3" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="B3">
         <v>190926</v>
@@ -1819,8 +2923,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>58</v>
+      <c r="A4" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="B4">
         <v>190926</v>
@@ -1848,8 +2952,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>59</v>
+      <c r="A5" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="B5">
         <v>190926</v>
@@ -1877,8 +2981,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>63</v>
+      <c r="A6" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="B6">
         <v>190926</v>
@@ -1906,8 +3010,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>65</v>
+      <c r="A7" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="B7">
         <v>190926</v>
@@ -1935,8 +3039,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>78</v>
+      <c r="A8" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="B8">
         <v>190926</v>
@@ -1964,8 +3068,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>61</v>
+      <c r="A9" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="B9">
         <v>190926</v>
@@ -1993,8 +3097,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>41</v>
+      <c r="A10" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="B10">
         <v>190926</v>
@@ -2022,8 +3126,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>44</v>
+      <c r="A11" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="B11">
         <v>190926</v>
@@ -2051,8 +3155,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>46</v>
+      <c r="A12" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="B12">
         <v>190926</v>
@@ -2080,8 +3184,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>49</v>
+      <c r="A13" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="B13">
         <v>190926</v>
@@ -2109,8 +3213,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>52</v>
+      <c r="A14" s="20" t="s">
+        <v>51</v>
       </c>
       <c r="B14">
         <v>190926</v>
@@ -2140,4 +3244,533 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" style="13" customWidth="1"/>
+    <col min="2" max="7" width="10.77734375" style="13" customWidth="1"/>
+    <col min="8" max="12" width="8.88671875" style="13" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update compustat raw data: currency USD only; Replicate Huang et al. 2014 Table 4
</commit_message>
<xml_diff>
--- a/output/Tables.xlsx
+++ b/output/Tables.xlsx
@@ -3116,154 +3116,154 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="55" t="inlineStr">
+      <c r="B1" s="70" t="inlineStr">
         <is>
           <t>count</t>
         </is>
       </c>
-      <c r="C1" s="55" t="inlineStr">
+      <c r="C1" s="70" t="inlineStr">
         <is>
           <t>mean</t>
         </is>
       </c>
-      <c r="D1" s="55" t="inlineStr">
+      <c r="D1" s="70" t="inlineStr">
         <is>
           <t>std</t>
         </is>
       </c>
-      <c r="E1" s="55" t="inlineStr">
+      <c r="E1" s="70" t="inlineStr">
         <is>
           <t>min</t>
         </is>
       </c>
-      <c r="F1" s="55" t="inlineStr">
+      <c r="F1" s="70" t="inlineStr">
         <is>
           <t>25%</t>
         </is>
       </c>
-      <c r="G1" s="55" t="inlineStr">
+      <c r="G1" s="70" t="inlineStr">
         <is>
           <t>50%</t>
         </is>
       </c>
-      <c r="H1" s="55" t="inlineStr">
+      <c r="H1" s="70" t="inlineStr">
         <is>
           <t>75%</t>
         </is>
       </c>
-      <c r="I1" s="55" t="inlineStr">
+      <c r="I1" s="70" t="inlineStr">
         <is>
           <t>max</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="55" t="inlineStr">
+      <c r="A2" s="70" t="inlineStr">
         <is>
           <t>NW</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C2" s="20" t="n">
-        <v>8.9979</v>
+        <v>8.998200000000001</v>
       </c>
       <c r="D2" s="20" t="n">
-        <v>0.7841</v>
+        <v>0.784</v>
       </c>
       <c r="E2" s="20" t="n">
         <v>7.044</v>
       </c>
       <c r="F2" s="20" t="n">
-        <v>8.458299999999999</v>
+        <v>8.4589</v>
       </c>
       <c r="G2" s="20" t="n">
-        <v>9.0685</v>
+        <v>9.0688</v>
       </c>
       <c r="H2" s="20" t="n">
-        <v>9.5388</v>
+        <v>9.5389</v>
       </c>
       <c r="I2" s="20" t="n">
         <v>13.49</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="55" t="inlineStr">
+      <c r="A3" s="70" t="inlineStr">
         <is>
           <t>nw</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C3" s="20" t="n">
-        <v>10884.8916</v>
+        <v>10887.4733</v>
       </c>
       <c r="D3" s="20" t="n">
-        <v>9969.416800000001</v>
+        <v>9968.7945</v>
       </c>
       <c r="E3" s="20" t="n">
         <v>1145</v>
       </c>
       <c r="F3" s="20" t="n">
-        <v>4713</v>
+        <v>4716</v>
       </c>
       <c r="G3" s="20" t="n">
-        <v>8677</v>
+        <v>8679</v>
       </c>
       <c r="H3" s="20" t="n">
-        <v>13887</v>
+        <v>13889</v>
       </c>
       <c r="I3" s="20" t="n">
         <v>722159</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="55" t="inlineStr">
+      <c r="A4" s="70" t="inlineStr">
         <is>
           <t>TONE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C4" s="20" t="n">
-        <v>-8.536799999999999</v>
+        <v>-8.5404</v>
       </c>
       <c r="D4" s="20" t="n">
-        <v>6.8003</v>
+        <v>6.8006</v>
       </c>
       <c r="E4" s="20" t="n">
         <v>-64.5429</v>
       </c>
       <c r="F4" s="20" t="n">
-        <v>-12.4361</v>
+        <v>-12.4408</v>
       </c>
       <c r="G4" s="20" t="n">
-        <v>-7.4335</v>
+        <v>-7.4363</v>
       </c>
       <c r="H4" s="20" t="n">
-        <v>-3.7419</v>
+        <v>-3.7453</v>
       </c>
       <c r="I4" s="20" t="n">
         <v>22.2874</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="55" t="inlineStr">
+      <c r="A5" s="70" t="inlineStr">
         <is>
           <t>TLAG</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C5" s="20" t="n">
-        <v>39.4541</v>
+        <v>39.4555</v>
       </c>
       <c r="D5" s="20" t="n">
-        <v>6.1783</v>
+        <v>6.1761</v>
       </c>
       <c r="E5" s="20" t="n">
         <v>0</v>
@@ -3282,19 +3282,19 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="55" t="inlineStr">
+      <c r="A6" s="70" t="inlineStr">
         <is>
           <t>RET</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C6" s="20" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0083</v>
       </c>
       <c r="D6" s="20" t="n">
-        <v>0.2856</v>
+        <v>0.2857</v>
       </c>
       <c r="E6" s="20" t="n">
         <v>-1.8331</v>
@@ -3306,20 +3306,20 @@
         <v>-0.0026</v>
       </c>
       <c r="H6" s="20" t="n">
-        <v>0.1276</v>
+        <v>0.1277</v>
       </c>
       <c r="I6" s="20" t="n">
         <v>18.3123</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="55" t="inlineStr">
+      <c r="A7" s="70" t="inlineStr">
         <is>
           <t>NEG</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C7" s="20" t="n">
         <v>0.5059</v>
@@ -3344,75 +3344,75 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="55" t="inlineStr">
+      <c r="A8" s="70" t="inlineStr">
         <is>
           <t>SIZE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C8" s="20" t="n">
-        <v>6.0071</v>
+        <v>6.0054</v>
       </c>
       <c r="D8" s="20" t="n">
-        <v>1.9804</v>
+        <v>1.9791</v>
       </c>
       <c r="E8" s="20" t="n">
-        <v>2.002</v>
+        <v>2.0016</v>
       </c>
       <c r="F8" s="20" t="n">
-        <v>4.5468</v>
+        <v>4.546</v>
       </c>
       <c r="G8" s="20" t="n">
-        <v>5.9069</v>
+        <v>5.9063</v>
       </c>
       <c r="H8" s="20" t="n">
-        <v>7.3064</v>
+        <v>7.3043</v>
       </c>
       <c r="I8" s="20" t="n">
-        <v>11.2053</v>
+        <v>11.2061</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="55" t="inlineStr">
+      <c r="A9" s="70" t="inlineStr">
         <is>
           <t>MTB</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C9" s="20" t="n">
-        <v>3.6475</v>
+        <v>3.6476</v>
       </c>
       <c r="D9" s="20" t="n">
-        <v>4.5019</v>
+        <v>4.505</v>
       </c>
       <c r="E9" s="20" t="n">
-        <v>0.2883</v>
+        <v>0.2881</v>
       </c>
       <c r="F9" s="20" t="n">
-        <v>1.356</v>
+        <v>1.3556</v>
       </c>
       <c r="G9" s="20" t="n">
-        <v>2.2624</v>
+        <v>2.2614</v>
       </c>
       <c r="H9" s="20" t="n">
-        <v>3.9946</v>
+        <v>3.9928</v>
       </c>
       <c r="I9" s="20" t="n">
-        <v>30.8754</v>
+        <v>30.9008</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="55" t="inlineStr">
+      <c r="A10" s="70" t="inlineStr">
         <is>
           <t>LEV</t>
         </is>
       </c>
       <c r="B10" s="21" t="n">
-        <v>190547</v>
+        <v>190341</v>
       </c>
       <c r="C10" s="20" t="n">
         <v>0.1975</v>
@@ -4164,54 +4164,54 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="55" t="inlineStr">
+      <c r="B1" s="70" t="inlineStr">
         <is>
           <t>NW</t>
         </is>
       </c>
-      <c r="C1" s="55" t="inlineStr">
+      <c r="C1" s="70" t="inlineStr">
         <is>
           <t>nw</t>
         </is>
       </c>
-      <c r="D1" s="55" t="inlineStr">
+      <c r="D1" s="70" t="inlineStr">
         <is>
           <t>TONE</t>
         </is>
       </c>
-      <c r="E1" s="55" t="inlineStr">
+      <c r="E1" s="70" t="inlineStr">
         <is>
           <t>TLAG</t>
         </is>
       </c>
-      <c r="F1" s="55" t="inlineStr">
+      <c r="F1" s="70" t="inlineStr">
         <is>
           <t>RET</t>
         </is>
       </c>
-      <c r="G1" s="55" t="inlineStr">
+      <c r="G1" s="70" t="inlineStr">
         <is>
           <t>NEG</t>
         </is>
       </c>
-      <c r="H1" s="55" t="inlineStr">
+      <c r="H1" s="70" t="inlineStr">
         <is>
           <t>SIZE</t>
         </is>
       </c>
-      <c r="I1" s="55" t="inlineStr">
+      <c r="I1" s="70" t="inlineStr">
         <is>
           <t>MTB</t>
         </is>
       </c>
-      <c r="J1" s="55" t="inlineStr">
+      <c r="J1" s="70" t="inlineStr">
         <is>
           <t>LEV</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="55" t="inlineStr">
+      <c r="A2" s="70" t="inlineStr">
         <is>
           <t>NW</t>
         </is>
@@ -4223,10 +4223,10 @@
         <v>0.8187</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.4452</v>
+        <v>-0.4453</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.2244</v>
+        <v>-0.2245</v>
       </c>
       <c r="F2" t="n">
         <v>-0.0186</v>
@@ -4235,17 +4235,17 @@
         <v>0.0076</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3295</v>
+        <v>0.3305</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0949</v>
+        <v>0.095</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0672</v>
+        <v>0.0667</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="55" t="inlineStr">
+      <c r="A3" s="70" t="inlineStr">
         <is>
           <t>nw</t>
         </is>
@@ -4257,97 +4257,97 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.3773</v>
+        <v>-0.3774</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1216</v>
+        <v>-0.1217</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0132</v>
+        <v>-0.0131</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0075</v>
+        <v>0.0074</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2336</v>
+        <v>0.2343</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0835</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0698</v>
+        <v>0.06950000000000001</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="55" t="inlineStr">
+      <c r="A4" s="70" t="inlineStr">
         <is>
           <t>TONE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.4546</v>
+        <v>-0.4547</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4546</v>
+        <v>-0.4547</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.017</v>
+        <v>0.0176</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0241</v>
+        <v>0.024</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0194</v>
+        <v>-0.0193</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0717</v>
+        <v>-0.07290000000000001</v>
       </c>
       <c r="I4" t="n">
         <v>-0.028</v>
       </c>
       <c r="J4" t="n">
-        <v>0.059</v>
+        <v>0.0592</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="55" t="inlineStr">
+      <c r="A5" s="70" t="inlineStr">
         <is>
           <t>TLAG</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2948</v>
+        <v>-0.2951</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2948</v>
+        <v>-0.2951</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0182</v>
+        <v>0.0189</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.031</v>
+        <v>-0.0309</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0455</v>
+        <v>0.0454</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.4097</v>
+        <v>-0.4093</v>
       </c>
       <c r="I5" t="n">
         <v>-0.0385</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.0273</v>
+        <v>-0.027</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="55" t="inlineStr">
+      <c r="A6" s="70" t="inlineStr">
         <is>
           <t>RET</t>
         </is>
@@ -4362,7 +4362,7 @@
         <v>0.0329</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.0521</v>
+        <v>-0.052</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -4371,7 +4371,7 @@
         <v>-0.6647</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0314</v>
+        <v>-0.0315</v>
       </c>
       <c r="I6" t="n">
         <v>-0.0189</v>
@@ -4381,7 +4381,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="55" t="inlineStr">
+      <c r="A7" s="70" t="inlineStr">
         <is>
           <t>NEG</t>
         </is>
@@ -4396,7 +4396,7 @@
         <v>-0.0227</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0451</v>
+        <v>0.045</v>
       </c>
       <c r="F7" t="n">
         <v>-0.866</v>
@@ -4415,90 +4415,90 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="55" t="inlineStr">
+      <c r="A8" s="70" t="inlineStr">
         <is>
           <t>SIZE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.3417</v>
+        <v>0.3424</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3417</v>
+        <v>0.3424</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0566</v>
+        <v>-0.0576</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.4235</v>
+        <v>-0.4231</v>
       </c>
       <c r="F8" t="n">
         <v>0.0156</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0274</v>
+        <v>-0.0273</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2332</v>
+        <v>0.2334</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1196</v>
+        <v>0.1198</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="55" t="inlineStr">
+      <c r="A9" s="70" t="inlineStr">
         <is>
           <t>MTB</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1145</v>
+        <v>0.1148</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1145</v>
+        <v>0.1148</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0143</v>
+        <v>0.014</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.09030000000000001</v>
+        <v>-0.0901</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0457</v>
+        <v>-0.0458</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0262</v>
+        <v>0.0263</v>
       </c>
       <c r="H9" t="n">
-        <v>0.398</v>
+        <v>0.3981</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.056</v>
+        <v>0.0561</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="55" t="inlineStr">
+      <c r="A10" s="70" t="inlineStr">
         <is>
           <t>LEV</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0572</v>
+        <v>0.0567</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0572</v>
+        <v>0.0567</v>
       </c>
       <c r="D10" t="n">
         <v>0.059</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0342</v>
+        <v>-0.034</v>
       </c>
       <c r="F10" t="n">
         <v>0.0023</v>
@@ -4507,10 +4507,10 @@
         <v>-0.0045</v>
       </c>
       <c r="H10" t="n">
-        <v>0.151</v>
+        <v>0.1509</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.0755</v>
+        <v>-0.07530000000000001</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -5346,7 +5346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
@@ -5410,25 +5410,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C2" s="20" t="n">
-        <v>8.9457</v>
+        <v>8.8596</v>
       </c>
       <c r="D2" s="20" t="n">
-        <v>0.7635999999999999</v>
+        <v>0.8035</v>
       </c>
       <c r="E2" s="20" t="n">
         <v>7.044</v>
       </c>
       <c r="F2" s="20" t="n">
-        <v>8.423500000000001</v>
+        <v>8.249599999999999</v>
       </c>
       <c r="G2" s="20" t="n">
-        <v>9.009600000000001</v>
+        <v>8.906499999999999</v>
       </c>
       <c r="H2" s="20" t="n">
-        <v>9.4771</v>
+        <v>9.423999999999999</v>
       </c>
       <c r="I2" s="20" t="n">
         <v>13.49</v>
@@ -5441,25 +5441,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C3" s="20" t="n">
-        <v>10214.6197</v>
+        <v>9766.9483</v>
       </c>
       <c r="D3" s="20" t="n">
-        <v>9672.1803</v>
+        <v>10329.6505</v>
       </c>
       <c r="E3" s="20" t="n">
         <v>1145</v>
       </c>
       <c r="F3" s="20" t="n">
-        <v>4552</v>
+        <v>3825</v>
       </c>
       <c r="G3" s="20" t="n">
-        <v>8180</v>
+        <v>7379</v>
       </c>
       <c r="H3" s="20" t="n">
-        <v>13056</v>
+        <v>12381</v>
       </c>
       <c r="I3" s="20" t="n">
         <v>722159</v>
@@ -5472,25 +5472,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C4" s="20" t="n">
-        <v>-8.456899999999999</v>
+        <v>-7.8206</v>
       </c>
       <c r="D4" s="20" t="n">
-        <v>6.8847</v>
+        <v>6.8046</v>
       </c>
       <c r="E4" s="20" t="n">
         <v>-64.5429</v>
       </c>
       <c r="F4" s="20" t="n">
-        <v>-12.4347</v>
+        <v>-11.5227</v>
       </c>
       <c r="G4" s="20" t="n">
-        <v>-7.4723</v>
+        <v>-6.8676</v>
       </c>
       <c r="H4" s="20" t="n">
-        <v>-3.6417</v>
+        <v>-3.182</v>
       </c>
       <c r="I4" s="20" t="n">
         <v>22.2874</v>
@@ -5503,13 +5503,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C5" s="20" t="n">
-        <v>39.0219</v>
+        <v>39.1049</v>
       </c>
       <c r="D5" s="20" t="n">
-        <v>6.2487</v>
+        <v>6.4114</v>
       </c>
       <c r="E5" s="20" t="n">
         <v>0</v>
@@ -5534,25 +5534,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C6" s="20" t="n">
-        <v>0.0182</v>
+        <v>0.0152</v>
       </c>
       <c r="D6" s="20" t="n">
-        <v>0.2531</v>
+        <v>0.2482</v>
       </c>
       <c r="E6" s="20" t="n">
         <v>-1.5787</v>
       </c>
       <c r="F6" s="20" t="n">
-        <v>-0.1126</v>
+        <v>-0.1125</v>
       </c>
       <c r="G6" s="20" t="n">
-        <v>0.0073</v>
+        <v>0.0048</v>
       </c>
       <c r="H6" s="20" t="n">
-        <v>0.1299</v>
+        <v>0.1237</v>
       </c>
       <c r="I6" s="20" t="n">
         <v>4.8492</v>
@@ -5565,13 +5565,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C7" s="20" t="n">
-        <v>0.4829</v>
+        <v>0.488</v>
       </c>
       <c r="D7" s="20" t="n">
-        <v>0.4997</v>
+        <v>0.4999</v>
       </c>
       <c r="E7" s="20" t="n">
         <v>0</v>
@@ -5596,28 +5596,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C8" s="20" t="n">
-        <v>6.4469</v>
+        <v>6.5224</v>
       </c>
       <c r="D8" s="20" t="n">
-        <v>1.7763</v>
+        <v>1.8596</v>
       </c>
       <c r="E8" s="20" t="n">
-        <v>2.002</v>
+        <v>2.0016</v>
       </c>
       <c r="F8" s="20" t="n">
-        <v>5.1751</v>
+        <v>5.1654</v>
       </c>
       <c r="G8" s="20" t="n">
-        <v>6.3171</v>
+        <v>6.3942</v>
       </c>
       <c r="H8" s="20" t="n">
-        <v>7.563</v>
+        <v>7.7139</v>
       </c>
       <c r="I8" s="20" t="n">
-        <v>11.2053</v>
+        <v>11.2061</v>
       </c>
     </row>
     <row r="9">
@@ -5627,28 +5627,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C9" s="20" t="n">
-        <v>3.5157</v>
+        <v>3.4871</v>
       </c>
       <c r="D9" s="20" t="n">
-        <v>4.0074</v>
+        <v>3.989</v>
       </c>
       <c r="E9" s="20" t="n">
-        <v>0.2883</v>
+        <v>0.2881</v>
       </c>
       <c r="F9" s="20" t="n">
-        <v>1.4855</v>
+        <v>1.4929</v>
       </c>
       <c r="G9" s="20" t="n">
-        <v>2.3436</v>
+        <v>2.3201</v>
       </c>
       <c r="H9" s="20" t="n">
-        <v>3.9028</v>
+        <v>3.8566</v>
       </c>
       <c r="I9" s="20" t="n">
-        <v>30.8754</v>
+        <v>30.9008</v>
       </c>
     </row>
     <row r="10">
@@ -5658,25 +5658,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C10" s="20" t="n">
-        <v>0.1924</v>
+        <v>0.2063</v>
       </c>
       <c r="D10" s="20" t="n">
-        <v>0.1821</v>
+        <v>0.1801</v>
       </c>
       <c r="E10" s="20" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="20" t="n">
-        <v>0.0106</v>
+        <v>0.0299</v>
       </c>
       <c r="G10" s="20" t="n">
-        <v>0.1623</v>
+        <v>0.1859</v>
       </c>
       <c r="H10" s="20" t="n">
-        <v>0.3151</v>
+        <v>0.327</v>
       </c>
       <c r="I10" s="20" t="n">
         <v>0.7242</v>
@@ -5689,28 +5689,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C11" s="20" t="n">
-        <v>0.043</v>
+        <v>0.0478</v>
       </c>
       <c r="D11" s="20" t="n">
-        <v>0.0664</v>
+        <v>0.0612</v>
       </c>
       <c r="E11" s="20" t="n">
         <v>-0.262</v>
       </c>
       <c r="F11" s="20" t="n">
-        <v>0.0226</v>
+        <v>0.0246</v>
       </c>
       <c r="G11" s="20" t="n">
-        <v>0.0485</v>
+        <v>0.0503</v>
       </c>
       <c r="H11" s="20" t="n">
-        <v>0.0732</v>
+        <v>0.0751</v>
       </c>
       <c r="I11" s="20" t="n">
-        <v>0.2275</v>
+        <v>0.2273</v>
       </c>
     </row>
     <row r="12">
@@ -5720,25 +5720,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C12" s="20" t="n">
-        <v>-0.0208</v>
+        <v>-0.021</v>
       </c>
       <c r="D12" s="20" t="n">
-        <v>0.0672</v>
+        <v>0.0669</v>
       </c>
       <c r="E12" s="20" t="n">
-        <v>-0.4449</v>
+        <v>-0.445</v>
       </c>
       <c r="F12" s="20" t="n">
-        <v>-0.0175</v>
+        <v>-0.0169</v>
       </c>
       <c r="G12" s="20" t="n">
-        <v>-0.0015</v>
+        <v>-0.0014</v>
       </c>
       <c r="H12" s="20" t="n">
-        <v>0.0024</v>
+        <v>0.0021</v>
       </c>
       <c r="I12" s="20" t="n">
         <v>0.0776</v>
@@ -5751,13 +5751,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C13" s="20" t="n">
-        <v>0.859</v>
+        <v>0.8584000000000001</v>
       </c>
       <c r="D13" s="20" t="n">
-        <v>0.4465</v>
+        <v>0.4533</v>
       </c>
       <c r="E13" s="20" t="n">
         <v>0.6931</v>
@@ -5782,13 +5782,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C14" s="20" t="n">
-        <v>0.8974</v>
+        <v>0.8927</v>
       </c>
       <c r="D14" s="20" t="n">
-        <v>0.5322</v>
+        <v>0.5312</v>
       </c>
       <c r="E14" s="20" t="n">
         <v>0.6931</v>
@@ -5813,25 +5813,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C15" s="20" t="n">
-        <v>8.311999999999999</v>
+        <v>8.3919</v>
       </c>
       <c r="D15" s="20" t="n">
-        <v>1.0327</v>
+        <v>1.0672</v>
       </c>
       <c r="E15" s="20" t="n">
         <v>5.8111</v>
       </c>
       <c r="F15" s="20" t="n">
-        <v>7.6353</v>
+        <v>7.6779</v>
       </c>
       <c r="G15" s="20" t="n">
-        <v>8.42</v>
+        <v>8.5337</v>
       </c>
       <c r="H15" s="20" t="n">
-        <v>9.0891</v>
+        <v>9.211499999999999</v>
       </c>
       <c r="I15" s="20" t="n">
         <v>10.2878</v>
@@ -5844,25 +5844,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C16" s="20" t="n">
-        <v>0.0046</v>
+        <v>0.008</v>
       </c>
       <c r="D16" s="20" t="n">
-        <v>0.0416</v>
+        <v>0.0376</v>
       </c>
       <c r="E16" s="20" t="n">
-        <v>-0.2006</v>
+        <v>-0.2005</v>
       </c>
       <c r="F16" s="20" t="n">
-        <v>0.0005</v>
+        <v>0.0026</v>
       </c>
       <c r="G16" s="20" t="n">
-        <v>0.0119</v>
+        <v>0.0131</v>
       </c>
       <c r="H16" s="20" t="n">
-        <v>0.0234</v>
+        <v>0.0245</v>
       </c>
       <c r="I16" s="20" t="n">
         <v>0.0843</v>
@@ -5875,25 +5875,25 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C17" s="20" t="n">
-        <v>0.0015</v>
+        <v>0.0017</v>
       </c>
       <c r="D17" s="20" t="n">
-        <v>0.0309</v>
+        <v>0.0292</v>
       </c>
       <c r="E17" s="20" t="n">
         <v>-0.1261</v>
       </c>
       <c r="F17" s="20" t="n">
-        <v>-0.0057</v>
+        <v>-0.0052</v>
       </c>
       <c r="G17" s="20" t="n">
         <v>0.0009</v>
       </c>
       <c r="H17" s="20" t="n">
-        <v>0.0075</v>
+        <v>0.0072</v>
       </c>
       <c r="I17" s="20" t="n">
         <v>0.1497</v>
@@ -5906,25 +5906,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C18" s="20" t="n">
-        <v>0.0199</v>
+        <v>0.0181</v>
       </c>
       <c r="D18" s="20" t="n">
-        <v>0.0301</v>
+        <v>0.028</v>
       </c>
       <c r="E18" s="20" t="n">
         <v>0.0009</v>
       </c>
       <c r="F18" s="20" t="n">
-        <v>0.0045</v>
+        <v>0.0042</v>
       </c>
       <c r="G18" s="20" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.0083</v>
       </c>
       <c r="H18" s="20" t="n">
-        <v>0.0209</v>
+        <v>0.0188</v>
       </c>
       <c r="I18" s="20" t="n">
         <v>0.1883</v>
@@ -5937,25 +5937,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C19" s="20" t="n">
-        <v>0.0887</v>
+        <v>0.0868</v>
       </c>
       <c r="D19" s="20" t="n">
-        <v>0.0696</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="E19" s="20" t="n">
         <v>0.0069</v>
       </c>
       <c r="F19" s="20" t="n">
-        <v>0.0404</v>
+        <v>0.0391</v>
       </c>
       <c r="G19" s="20" t="n">
-        <v>0.0699</v>
+        <v>0.0679</v>
       </c>
       <c r="H19" s="20" t="n">
-        <v>0.1153</v>
+        <v>0.1128</v>
       </c>
       <c r="I19" s="20" t="n">
         <v>0.3787</v>
@@ -5968,13 +5968,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C20" s="20" t="n">
-        <v>0.2424</v>
+        <v>0.2057</v>
       </c>
       <c r="D20" s="20" t="n">
-        <v>0.4285</v>
+        <v>0.4042</v>
       </c>
       <c r="E20" s="20" t="n">
         <v>0</v>
@@ -5999,28 +5999,59 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>91627</v>
+        <v>53218</v>
       </c>
       <c r="C21" s="20" t="n">
-        <v>-0.0005</v>
+        <v>0</v>
       </c>
       <c r="D21" s="20" t="n">
-        <v>6.5766</v>
+        <v>6.5029</v>
       </c>
       <c r="E21" s="20" t="n">
-        <v>-57.6576</v>
+        <v>-58.0504</v>
       </c>
       <c r="F21" s="20" t="n">
-        <v>-3.7479</v>
+        <v>-3.4931</v>
       </c>
       <c r="G21" s="20" t="n">
-        <v>0.8705000000000001</v>
+        <v>0.8804999999999999</v>
       </c>
       <c r="H21" s="20" t="n">
-        <v>4.5628</v>
+        <v>4.4065</v>
       </c>
       <c r="I21" s="20" t="n">
-        <v>31.5243</v>
+        <v>30.8696</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="70" t="inlineStr">
+        <is>
+          <t>DA</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>53218</v>
+      </c>
+      <c r="C22" t="n">
+        <v>38.3977</v>
+      </c>
+      <c r="D22" t="n">
+        <v>269.699</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-1096.6013</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-17.6796</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.6611</v>
+      </c>
+      <c r="H22" t="n">
+        <v>25.9003</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1578.0097</v>
       </c>
     </row>
   </sheetData>
@@ -6034,7 +6065,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6146,6 +6177,11 @@
           <t>ABTONE</t>
         </is>
       </c>
+      <c r="V1" s="70" t="inlineStr">
+        <is>
+          <t>DA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="70" t="inlineStr">
@@ -6157,61 +6193,64 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.792</v>
+        <v>0.7796999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.4614</v>
+        <v>-0.4583</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.195</v>
+        <v>-0.2061</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.0076</v>
+        <v>-0.0031</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0032</v>
+        <v>-0.0043</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2576</v>
+        <v>0.2852</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0586</v>
+        <v>0.0453</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0367</v>
+        <v>0.07480000000000001</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.0672</v>
+        <v>-0.0239</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0122</v>
+        <v>-0.0002</v>
       </c>
       <c r="M2" t="n">
-        <v>0.238</v>
+        <v>0.2672</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2583</v>
+        <v>0.284</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.0376</v>
+        <v>-0.0197</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.1153</v>
+        <v>-0.0877</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0014</v>
+        <v>0.0018</v>
       </c>
       <c r="R2" t="n">
-        <v>0.08989999999999999</v>
+        <v>0.0745</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.0336</v>
+        <v>-0.0436</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1277</v>
+        <v>0.1086</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.3842</v>
+        <v>-0.3714</v>
+      </c>
+      <c r="V2" t="n">
+        <v>-0.0037</v>
       </c>
     </row>
     <row r="3">
@@ -6227,58 +6266,61 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.3498</v>
+        <v>-0.3373</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.0926</v>
+        <v>-0.0888</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0121</v>
+        <v>-0.0122</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0097</v>
+        <v>0.0072</v>
       </c>
       <c r="H3" t="n">
         <v>0.1665</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0479</v>
+        <v>0.0361</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0488</v>
+        <v>0.0675</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0535</v>
+        <v>-0.0241</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0051</v>
+        <v>-0.0039</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1453</v>
+        <v>0.1541</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1617</v>
+        <v>0.1693</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.0564</v>
+        <v>-0.0532</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.0684</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.0015</v>
+        <v>-0.0035</v>
       </c>
       <c r="R3" t="n">
-        <v>0.06660000000000001</v>
+        <v>0.0562</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.0144</v>
+        <v>-0.0168</v>
       </c>
       <c r="T3" t="n">
-        <v>0.0922</v>
+        <v>0.081</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.2981</v>
+        <v>-0.2831</v>
+      </c>
+      <c r="V3" t="n">
+        <v>-0.0182</v>
       </c>
     </row>
     <row r="4">
@@ -6288,64 +6330,67 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.4859</v>
+        <v>-0.4878</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4859</v>
+        <v>-0.4878</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0253</v>
+        <v>0.0374</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0206</v>
+        <v>0.0169</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0211</v>
+        <v>-0.0155</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0697</v>
+        <v>-0.091</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.016</v>
+        <v>-0.0116</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06909999999999999</v>
+        <v>0.0337</v>
       </c>
       <c r="K4" t="n">
-        <v>0.06950000000000001</v>
+        <v>0.0335</v>
       </c>
       <c r="L4" t="n">
-        <v>0.098</v>
+        <v>0.1045</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.0336</v>
+        <v>-0.0594</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0696</v>
+        <v>-0.1069</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0538</v>
+        <v>0.025</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1558</v>
+        <v>0.1406</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.0019</v>
+        <v>-0.0022</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.144</v>
+        <v>-0.1276</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.08119999999999999</v>
+        <v>-0.06419999999999999</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.2147</v>
+        <v>-0.1919</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9553</v>
+        <v>0.9557</v>
+      </c>
+      <c r="V4" t="n">
+        <v>-0.0226</v>
       </c>
     </row>
     <row r="5">
@@ -6355,64 +6400,67 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2662</v>
+        <v>-0.2817</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2662</v>
+        <v>-0.2817</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0291</v>
+        <v>0.0443</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.0224</v>
+        <v>-0.0262</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0343</v>
+        <v>0.0406</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.3309</v>
+        <v>-0.3343</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0217</v>
+        <v>-0.0115</v>
       </c>
       <c r="J5" t="n">
-        <v>0.009299999999999999</v>
+        <v>0.0161</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.09229999999999999</v>
+        <v>-0.0883</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1273</v>
+        <v>-0.1227</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.2294</v>
+        <v>-0.2428</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.2457</v>
+        <v>-0.2619</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.2285</v>
+        <v>-0.2287</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.1367</v>
+        <v>-0.1304</v>
       </c>
       <c r="Q5" t="n">
         <v>-0.0046</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1212</v>
+        <v>0.1254</v>
       </c>
       <c r="S5" t="n">
-        <v>0.1893</v>
+        <v>0.1826</v>
       </c>
       <c r="T5" t="n">
-        <v>0.1462</v>
+        <v>0.134</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0196</v>
+        <v>0.0109</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-0.063</v>
       </c>
     </row>
     <row r="6">
@@ -6422,65 +6470,68 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.008</v>
+        <v>0.0013</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.008</v>
+        <v>0.0013</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0289</v>
+        <v>0.0251</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.0325</v>
+        <v>-0.0404</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.6841</v>
+        <v>-0.6808</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0643</v>
+        <v>-0.0481</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0259</v>
+        <v>-0.0123</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0021</v>
+        <v>-0.0017</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0181</v>
+        <v>-0.0436</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1547</v>
+        <v>0.1637</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0124</v>
+        <v>-0.0119</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0209</v>
+        <v>-0.0205</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0019</v>
+        <v>0.0012</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0636</v>
+        <v>0.0698</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0362</v>
+        <v>0.0467</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0105</v>
+        <v>0.0168</v>
       </c>
       <c r="S6" t="n">
-        <v>0.266</v>
+        <v>0.2689</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0679</v>
+        <v>-0.0698</v>
       </c>
       <c r="U6" t="n">
         <v>-0</v>
       </c>
+      <c r="V6" t="n">
+        <v>0.0101</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="70" t="inlineStr">
@@ -6489,64 +6540,67 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0044</v>
+        <v>-0.0051</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0044</v>
+        <v>-0.0051</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0242</v>
+        <v>-0.0183</v>
       </c>
       <c r="E7" t="n">
-        <v>0.033</v>
+        <v>0.039</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.8655</v>
+        <v>-0.8658</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0001</v>
+        <v>-0.0101</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0125</v>
+        <v>0.0074</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0019</v>
+        <v>0.0007</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0151</v>
+        <v>0.0321</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.1242</v>
+        <v>-0.1318</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0008</v>
+        <v>-0.0008</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0119</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.018</v>
+        <v>-0.0209</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.07140000000000001</v>
+        <v>-0.0786</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0188</v>
+        <v>-0.0272</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0159</v>
+        <v>0.0126</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.1176</v>
+        <v>-0.1174</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0779</v>
+        <v>0.07969999999999999</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.0001</v>
+        <v>0.0022</v>
+      </c>
+      <c r="V7" t="n">
+        <v>-0.0238</v>
       </c>
     </row>
     <row r="8">
@@ -6556,64 +6610,67 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2664</v>
+        <v>0.3043</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2664</v>
+        <v>0.3043</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0526</v>
+        <v>-0.0819</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.3327</v>
+        <v>-0.3401</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.024</v>
+        <v>-0.0059</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0011</v>
+        <v>-0.0117</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2335</v>
+        <v>0.2502</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0998</v>
+        <v>0.0733</v>
       </c>
       <c r="K8" t="n">
-        <v>0.077</v>
+        <v>0.0317</v>
       </c>
       <c r="L8" t="n">
-        <v>0.2696</v>
+        <v>0.2843</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1976</v>
+        <v>0.2095</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2151</v>
+        <v>0.2267</v>
       </c>
       <c r="O8" t="n">
-        <v>0.3441</v>
+        <v>0.3741</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2588</v>
+        <v>0.2494</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.0235</v>
+        <v>-0.0234</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1976</v>
+        <v>-0.2015</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.31</v>
+        <v>-0.3148</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.2634</v>
+        <v>-0.2495</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.1768</v>
       </c>
     </row>
     <row r="9">
@@ -6623,64 +6680,67 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0482</v>
+        <v>0.0328</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0482</v>
+        <v>0.0328</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0373</v>
+        <v>0.0441</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0419</v>
+        <v>-0.0306</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0547</v>
+        <v>-0.0414</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0329</v>
+        <v>0.0252</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3817</v>
+        <v>0.3931</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0456</v>
+        <v>0.0431</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.1562</v>
+        <v>-0.1652</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1202</v>
+        <v>0.1156</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0051</v>
+        <v>-0.0091</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0028</v>
+        <v>-0.009900000000000001</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.08840000000000001</v>
+        <v>-0.0859</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0412</v>
+        <v>-0.0119</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0222</v>
+        <v>0.0181</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1585</v>
+        <v>0.1644</v>
       </c>
       <c r="S9" t="n">
-        <v>0.0359</v>
+        <v>0.0486</v>
       </c>
       <c r="T9" t="n">
-        <v>0.0343</v>
+        <v>0.0212</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.0355</v>
       </c>
     </row>
     <row r="10">
@@ -6690,64 +6750,67 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0148</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0148</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0746</v>
+        <v>0.0264</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0005</v>
+        <v>-0.0002</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0031</v>
+        <v>0.0011</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.0041</v>
+        <v>-0.0021</v>
       </c>
       <c r="H10" t="n">
-        <v>0.143</v>
+        <v>0.1187</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.1112</v>
+        <v>-0.1113</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.1669</v>
+        <v>0.1544</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.0683</v>
+        <v>-0.06560000000000001</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0348</v>
+        <v>0.0295</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.0052</v>
+        <v>-0.0117</v>
       </c>
       <c r="O10" t="n">
-        <v>0.1011</v>
+        <v>0.08119999999999999</v>
       </c>
       <c r="P10" t="n">
-        <v>0.0394</v>
+        <v>0.0045</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0339</v>
+        <v>0.036</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.1245</v>
+        <v>-0.1111</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.0721</v>
+        <v>-0.06519999999999999</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.0583</v>
+        <v>-0.0296</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0682</v>
+        <v>0.0407</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.0077</v>
       </c>
     </row>
     <row r="11">
@@ -6757,64 +6820,67 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.0171</v>
+        <v>0.0248</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0171</v>
+        <v>0.0248</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0605</v>
+        <v>0.0164</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.1247</v>
+        <v>-0.121</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.08649999999999999</v>
+        <v>-0.1052</v>
       </c>
       <c r="G11" t="n">
-        <v>0.07149999999999999</v>
+        <v>0.0834</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0254</v>
+        <v>-0.0154</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.2992</v>
+        <v>-0.3062</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2509</v>
+        <v>0.2257</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.057</v>
+        <v>0.0654</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0683</v>
+        <v>0.06469999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0793</v>
+        <v>0.0703</v>
       </c>
       <c r="O11" t="n">
-        <v>0.2021</v>
+        <v>0.175</v>
       </c>
       <c r="P11" t="n">
-        <v>0.4722</v>
+        <v>0.3881</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0161</v>
+        <v>0.0145</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.2565</v>
+        <v>-0.216</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.1452</v>
+        <v>-0.1202</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.4101</v>
+        <v>-0.3479</v>
       </c>
       <c r="U11" t="n">
-        <v>0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.0292</v>
       </c>
     </row>
     <row r="12">
@@ -6824,65 +6890,68 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0398</v>
+        <v>0.0172</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0398</v>
+        <v>0.0172</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0969</v>
+        <v>0.1097</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.149</v>
+        <v>-0.1378</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1807</v>
+        <v>0.1953</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.1573</v>
+        <v>-0.1694</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2314</v>
+        <v>0.2366</v>
       </c>
       <c r="I12" t="n">
-        <v>0.226</v>
+        <v>0.2319</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.0522</v>
+        <v>-0.0594</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0602</v>
+        <v>0.0486</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0508</v>
+        <v>0.0482</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0441</v>
+        <v>0.0401</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0717</v>
+        <v>0.098</v>
       </c>
       <c r="P12" t="n">
-        <v>0.2408</v>
+        <v>0.2766</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0044</v>
+        <v>0.0046</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.1431</v>
+        <v>-0.1567</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.1586</v>
+        <v>-0.1692</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.3151</v>
+        <v>-0.3488</v>
       </c>
       <c r="U12" t="n">
         <v>-0</v>
       </c>
+      <c r="V12" t="n">
+        <v>0.0455</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="70" t="inlineStr">
@@ -6891,64 +6960,67 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.2826</v>
+        <v>0.322</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2826</v>
+        <v>0.322</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.0472</v>
+        <v>-0.08110000000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.2681</v>
+        <v>-0.2878</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.0053</v>
+        <v>-0.0031</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.0001</v>
+        <v>-0.0013</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1802</v>
+        <v>0.2013</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0271</v>
+        <v>0.0195</v>
       </c>
       <c r="J13" t="n">
-        <v>0.011</v>
+        <v>0.0152</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0896</v>
+        <v>0.0924</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0215</v>
+        <v>0.0195</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.7123</v>
+        <v>0.7201</v>
       </c>
       <c r="O13" t="n">
-        <v>0.1414</v>
+        <v>0.1327</v>
       </c>
       <c r="P13" t="n">
-        <v>0.0354</v>
+        <v>0.0311</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.0055</v>
+        <v>-0.0038</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.0568</v>
+        <v>-0.0565</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.1491</v>
+        <v>-0.1521</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.0408</v>
+        <v>-0.0325</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.0484</v>
       </c>
     </row>
     <row r="14">
@@ -6958,64 +7030,67 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.2988</v>
+        <v>0.3335</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2988</v>
+        <v>0.3335</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.06510000000000001</v>
+        <v>-0.1022</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.2862</v>
+        <v>-0.3056</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0151</v>
+        <v>-0.0128</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2156</v>
+        <v>0.2298</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0171</v>
+        <v>0.0168</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0104</v>
+        <v>0.0058</v>
       </c>
       <c r="K14" t="n">
-        <v>0.1178</v>
+        <v>0.1098</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0187</v>
+        <v>0.0119</v>
       </c>
       <c r="M14" t="n">
-        <v>0.7976</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>0.1455</v>
+        <v>0.1404</v>
       </c>
       <c r="P14" t="n">
-        <v>0.0462</v>
+        <v>0.0288</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.0065</v>
+        <v>-0.0024</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.06660000000000001</v>
+        <v>-0.0571</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.1527</v>
+        <v>-0.1521</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0346</v>
+        <v>-0.0156</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.0493</v>
       </c>
     </row>
     <row r="15">
@@ -7025,64 +7100,67 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.0313</v>
+        <v>-0.0005999999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.0313</v>
+        <v>-0.0005999999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0597</v>
+        <v>0.0259</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.2318</v>
+        <v>-0.2368</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0115</v>
+        <v>0.0158</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.0151</v>
+        <v>-0.0191</v>
       </c>
       <c r="H15" t="n">
-        <v>0.3362</v>
+        <v>0.3822</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.08069999999999999</v>
+        <v>-0.0524</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1464</v>
+        <v>0.1254</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2107</v>
+        <v>0.1843</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0598</v>
+        <v>0.0819</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1246</v>
+        <v>0.1136</v>
       </c>
       <c r="N15" t="n">
-        <v>0.152</v>
+        <v>0.1416</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>0.2108</v>
+        <v>0.194</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.0038</v>
+        <v>0.0024</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.2236</v>
+        <v>-0.2357</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.2622</v>
+        <v>-0.2781</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.2215</v>
+        <v>-0.2147</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.0953</v>
       </c>
     </row>
     <row r="16">
@@ -7092,64 +7170,67 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.1374</v>
+        <v>-0.1134</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.1374</v>
+        <v>-0.1134</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2231</v>
+        <v>0.2071</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.1464</v>
+        <v>-0.1308</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1141</v>
+        <v>0.1219</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0979</v>
+        <v>-0.1023</v>
       </c>
       <c r="H16" t="n">
-        <v>0.2991</v>
+        <v>0.2802</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2816</v>
+        <v>0.3335</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.0731</v>
+        <v>-0.1377</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2468</v>
+        <v>0.1651</v>
       </c>
       <c r="L16" t="n">
-        <v>0.3567</v>
+        <v>0.3893</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0027</v>
+        <v>-0.0039</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0233</v>
+        <v>0.0068</v>
       </c>
       <c r="O16" t="n">
-        <v>0.1718</v>
+        <v>0.1462</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.3017</v>
+        <v>0.3203</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.4117</v>
+        <v>-0.3947</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.2294</v>
+        <v>-0.2141</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.6895</v>
+        <v>-0.6786</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.0813</v>
       </c>
     </row>
     <row r="17">
@@ -7159,64 +7240,67 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0049</v>
+        <v>0.005</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0049</v>
+        <v>0.005</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0121</v>
+        <v>0.0141</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.0136</v>
+        <v>-0.0158</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0594</v>
+        <v>0.06909999999999999</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.0411</v>
+        <v>-0.05</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.0133</v>
+        <v>-0.0061</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0188</v>
+        <v>0.0288</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0239</v>
+        <v>0.0256</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0157</v>
+        <v>0.0135</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0906</v>
+        <v>0.0917</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.0098</v>
+        <v>-0.0057</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.0061</v>
+        <v>-0.0016</v>
       </c>
       <c r="O17" t="n">
-        <v>0.0026</v>
+        <v>0.0027</v>
       </c>
       <c r="P17" t="n">
-        <v>0.2991</v>
+        <v>0.3182</v>
       </c>
       <c r="Q17" t="n">
         <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>0.0547</v>
+        <v>0.0664</v>
       </c>
       <c r="S17" t="n">
-        <v>0.0148</v>
+        <v>0.0167</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.1665</v>
+        <v>-0.1809</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.0398</v>
       </c>
     </row>
     <row r="18">
@@ -7226,64 +7310,67 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.089</v>
+        <v>0.0623</v>
       </c>
       <c r="C18" t="n">
-        <v>0.089</v>
+        <v>0.0623</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.1911</v>
+        <v>-0.1645</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1527</v>
+        <v>0.1501</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.0239</v>
+        <v>-0.0209</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0281</v>
+        <v>0.0235</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.2808</v>
+        <v>-0.275</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0935</v>
+        <v>0.0805</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.2005</v>
+        <v>-0.1739</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.2051</v>
+        <v>-0.1429</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.1526</v>
+        <v>-0.1634</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.0601</v>
+        <v>-0.0562</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.07240000000000001</v>
+        <v>-0.0587</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.2497</v>
+        <v>-0.2565</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.2754</v>
+        <v>-0.2228</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.0357</v>
+        <v>0.0433</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>0.2414</v>
+        <v>0.2452</v>
       </c>
       <c r="T18" t="n">
-        <v>0.3552</v>
+        <v>0.3443</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>-0.0525</v>
       </c>
     </row>
     <row r="19">
@@ -7293,65 +7380,68 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.0508</v>
+        <v>-0.0674</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.0508</v>
+        <v>-0.0674</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.07729999999999999</v>
+        <v>-0.0587</v>
       </c>
       <c r="E19" t="n">
-        <v>0.214</v>
+        <v>0.212</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1281</v>
+        <v>0.1225</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.08799999999999999</v>
+        <v>-0.0856</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.325</v>
+        <v>-0.3353</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.0408</v>
+        <v>-0.0456</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.1025</v>
+        <v>-0.09420000000000001</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.1313</v>
+        <v>-0.1065</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.1103</v>
+        <v>-0.1188</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.1606</v>
+        <v>-0.1685</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.1791</v>
+        <v>-0.18</v>
       </c>
       <c r="O19" t="n">
-        <v>-0.2745</v>
+        <v>-0.2907</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.1875</v>
+        <v>-0.1678</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.0035</v>
+        <v>0.0032</v>
       </c>
       <c r="R19" t="n">
-        <v>0.2774</v>
+        <v>0.271</v>
       </c>
       <c r="S19" t="n">
         <v>1</v>
       </c>
       <c r="T19" t="n">
-        <v>0.2422</v>
+        <v>0.2358</v>
       </c>
       <c r="U19" t="n">
         <v>-0</v>
       </c>
+      <c r="V19" t="n">
+        <v>-0.0579</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="70" t="inlineStr">
@@ -7360,64 +7450,67 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1282</v>
+        <v>0.1056</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1282</v>
+        <v>0.1056</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.2283</v>
+        <v>-0.2068</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1432</v>
+        <v>0.1331</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.0898</v>
+        <v>-0.0936</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0779</v>
+        <v>0.07969999999999999</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.2689</v>
+        <v>-0.2537</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.0569</v>
+        <v>-0.07539999999999999</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.0926</v>
+        <v>-0.0616</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.358</v>
+        <v>-0.2903</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.2761</v>
+        <v>-0.2998</v>
       </c>
       <c r="M20" t="n">
-        <v>-0.0148</v>
+        <v>-0.0092</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.0349</v>
+        <v>-0.0146</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.2244</v>
+        <v>-0.2171</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.7422</v>
+        <v>-0.7002</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.2052</v>
+        <v>-0.2196</v>
       </c>
       <c r="R20" t="n">
-        <v>0.4306</v>
+        <v>0.4016</v>
       </c>
       <c r="S20" t="n">
-        <v>0.2261</v>
+        <v>0.2152</v>
       </c>
       <c r="T20" t="n">
         <v>1</v>
       </c>
       <c r="U20" t="n">
-        <v>-0.0001</v>
+        <v>-0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>-0.08210000000000001</v>
       </c>
     </row>
     <row r="21">
@@ -7427,63 +7520,136 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.4005</v>
+        <v>-0.3884</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.4005</v>
+        <v>-0.3884</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9421</v>
+        <v>0.9393</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0205</v>
+        <v>0.0145</v>
       </c>
       <c r="F21" t="n">
         <v>0.0011</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.0014</v>
+        <v>0.0011</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0189</v>
+        <v>0.0131</v>
       </c>
       <c r="I21" t="n">
-        <v>0.06320000000000001</v>
+        <v>0.062</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0751</v>
+        <v>0.037</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0032</v>
+        <v>-0.01</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0246</v>
+        <v>0.0331</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.0037</v>
+        <v>-0.009900000000000001</v>
       </c>
       <c r="N21" t="n">
-        <v>0.0019</v>
+        <v>0.0021</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0059</v>
+        <v>0.0024</v>
       </c>
       <c r="P21" t="n">
-        <v>0.0634</v>
+        <v>0.0655</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.0089</v>
+        <v>-0.0047</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.0659</v>
+        <v>-0.0576</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.0121</v>
+        <v>-0.0111</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.0043</v>
+        <v>-0.0013</v>
       </c>
       <c r="U21" t="n">
+        <v>1</v>
+      </c>
+      <c r="V21" t="n">
+        <v>-0.0132</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="70" t="inlineStr">
+        <is>
+          <t>DA</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-0.075</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.075</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0332</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.0015</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0312</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.0292</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-0.0136</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0241</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-0.06270000000000001</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.009599999999999999</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.0067</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.1084</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.0863</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-0.0195</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="T22" t="n">
+        <v>-0.1011</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="V22" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>